<commit_message>
adding filtering by cluster
</commit_message>
<xml_diff>
--- a/faculty_unique_mesh_terms.xlsx
+++ b/faculty_unique_mesh_terms.xlsx
@@ -453,7 +453,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Adaptation, Physiological; Australia; Authorship; Bacteria; Biodegradation, Environmental; Biological Evolution; Biomass; California; Carbon; Carbon Cycle; Climate; Climate Change; Communication; Conservation of Natural Resources; Coral Reefs; Curriculum; Drought Resistance; Droughts; Ecological and Environmental Phenomena; Ecosystem; Education, Graduate; Environmental Justice; Environmental Microbiology; Environmental Science; Enzymes; Extreme Weather; Financial Management; Forests; Genomics; Grassland; Greenhouse Gases; Humanities; Interdisciplinary Communication; Introduced Species; Isoptera; Life History Traits; Loma; Metagenome; Metagenomics; Methane; Microbial Interactions; Microbiota; Mutation; Nitrification; Nitrogen; Phylogeny; Plant Leaves; Plants; Policy; Policy Making; Program Evaluation; Resilience, Psychological; Skin Pigmentation; Social Sciences; Soil; Soil Microbiology; Sphingomonas; Stress, Physiological; Temperature; Trees; Tropical Climate; Uncertainty; Water; Wildfires; Wood; Workforce; Writing; nan</t>
+          <t>Adaptation, Physiological; Australia; Authorship; Bacteria; Biodegradation, Environmental; Biological Evolution; Biomass; California; Carbon; Carbon Cycle; Climate; Climate Change; Communication; Conservation of Natural Resources; Coral Reefs; Curriculum; Drought Resistance; Droughts; Ecological and Environmental Phenomena; Ecosystem; Education, Graduate; Environmental Justice; Environmental Microbiology; Environmental Science; Enzymes; Extreme Weather; Feasibility Studies; Financial Management; Forests; Genomics; Government; Government Agencies; Grassland; Greenhouse Gases; Hot Temperature; Humanities; Interdisciplinary Communication; Interdisciplinary Research; Introduced Species; Isoptera; Life History Traits; Loma; Metagenome; Metagenomics; Methane; Microbial Interactions; Microbiota; Mutation; Needs Assessment; Nitrification; Nitrogen; Phylogeny; Plant Leaves; Plants; Policy; Policy Making; Private Sector; Program Evaluation; Resilience, Psychological; Risk Assessment; Skin Pigmentation; Social Planning; Social Sciences; Soil; Soil Microbiology; Sphingomonas; Stress, Physiological; Temperature; Trees; Tropical Climate; Uncertainty; Water; Wildfires; Wood; Workforce; Writing</t>
         </is>
       </c>
     </row>
@@ -537,7 +537,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Acetylation; Administration, Inhalation; Aged; Aging; Alleles; Alzheimer Disease; Amino Acid Sequence; Amyloid beta-Peptides; Amyloidogenic Proteins; Amyloidosis; Antibodies; Antibodies, Monoclonal; Apolipoprotein E3; Apolipoprotein E4; Apolipoproteins E; Astrocytes; Autoimmune Diseases; Biomarkers; Blood-Brain Barrier; Brain; Brain Injuries, Traumatic; Brain Neoplasms; Breast Neoplasms; C9orf72 Protein; Calcinosis; Calcium; Calcium Signaling; Caregivers; Cell Death; Cell Movement; Cell- and Tissue-Based Therapy; Cells, Cultured; Chemokines; Chemotaxis; Chimera; Cholesterol; Chromatin; Chromatin Immunoprecipitation Sequencing; Coculture Techniques; Cognition; Cognitive Dysfunction; Complement C1q; Contusions; Cyclic AMP; Cytokines; Dementia; Diabetes Mellitus; Diet; Disease Progression; Drug Development; Endoplasmic Reticulum; Endosomal Sorting Complexes Required for Transport; Endothelial Cells; Epigenesis, Genetic; Ferroptosis; Frontal Lobe; Frontotemporal Dementia; Gene Expression; Gene Expression Profiling; Gene Expression Regulation; Gene Regulatory Networks; Genome-Wide Association Study; Genomics; Gliosis; Grassland; Hippocampus; Histones; Homeostasis; Housing Quality; Immunohistochemistry; Immunotherapy; Induced Pluripotent Stem Cells; Infant; Infant, Newborn; Inflammation; Inflammation Mediators; Injections, Intraperitoneal; Interferon-gamma; Interferons; Interleukin-17; Interleukin-1beta; Intermediate Filaments; Intracranial Hemorrhages; Isothiocyanates; Leukoencephalopathies; Lipid Metabolism; Lipid Peroxidation; Lipopolysaccharides; Liver Diseases; Lysosomes; Macrophage Colony-Stimulating Factor; Macrophages; Microglia; Microscopy; Microtubules; Mitochondria; Monocytes; Multiple Sclerosis; Mutation; Mycoses; Myelin Basic Protein; Myelin Sheath; Myeloid Cells; NF-E2-Related Factor 2; Nervous System Diseases; Nervous System Malformations; Neurites; Neurodegenerative Diseases; Neurofibrillary Tangles; Neuroinflammatory Diseases; Neurons; Neutrophils; Nucleotide Motifs; Obesity; Organelles; Organic Chemicals; Organoids; Outcome Assessment, Health Care; Oxidative Stress; Parkinson Disease; Patient Advocacy; Phagocytosis; Phenotype; Phosphorylation; Physicians; Pick Disease of the Brain; Plaque, Amyloid; Pluripotent Stem Cells; Presenilin-1; Prosencephalon; Protein Isoforms; Proteomics; Quantitative Trait Loci; RNA; Rare Diseases; Receptor, Macrophage Colony-Stimulating Factor; Receptors, Chimeric Antigen; Receptors, Granulocyte-Macrophage Colony-Stimulating Factor; Research Report; Resilience, Psychological; Risk Factors; Schizophrenia; Sequence Analysis, RNA; Sex Factors; Single-Cell Gene Expression Analysis; Social Cohesion; Stem Cell Research; Stem Cells; Sulfoxides; Synaptophysin; Tauopathies; Thalamus; Tissue Distribution; Toll-Like Receptor 4; Transcription Factors; Transcriptional Activation; Transcriptome; Transplantation, Heterologous; Treatment Outcome; Twins, Monozygotic; Weaning; White Matter; Whole Genome Sequencing; Xenon; anti-synaptophysin; heparin proteoglycan; peptide A; tau Proteins</t>
+          <t>Acetylation; Administration, Inhalation; Aged; Aging; Alleles; Alzheimer Disease; Amino Acid Sequence; Amyloid beta-Peptides; Amyloidogenic Proteins; Amyloidosis; Antibodies; Antibodies, Monoclonal; Apolipoprotein E3; Apolipoprotein E4; Apolipoproteins E; Astrocytes; Autoimmune Diseases; Biomarkers; Blood-Brain Barrier; Brain; Brain Injuries, Traumatic; Brain Neoplasms; Breast Neoplasms; C9orf72 Protein; Calcinosis; Calcium; Calcium Signaling; Caregivers; Cell Death; Cell Movement; Cell- and Tissue-Based Therapy; Cells, Cultured; Chemokines; Chemotaxis; Chimera; Cholesterol; Chromatin; Chromatin Immunoprecipitation Sequencing; Coculture Techniques; Cognition; Cognitive Dysfunction; Complement C1q; Contusions; Cyclic AMP; Cytokines; Dementia; Diabetes Mellitus; Diet; Disease Progression; Drug Development; Endoplasmic Reticulum; Endosomal Sorting Complexes Required for Transport; Endothelial Cells; Epigenesis, Genetic; Ferroptosis; Frontal Lobe; Frontotemporal Dementia; Gene Expression; Gene Expression Profiling; Gene Expression Regulation; Gene Regulatory Networks; Genome-Wide Association Study; Genomics; Gliosis; Grassland; Hepatitis A Virus Cellular Receptor 2; Hippocampus; Histones; Homeostasis; Housing Quality; Immunohistochemistry; Immunotherapy; Induced Pluripotent Stem Cells; Infant; Infant, Newborn; Inflammation; Inflammation Mediators; Injections, Intraperitoneal; Interferon-gamma; Interferons; Interleukin-17; Interleukin-1beta; Intermediate Filaments; Intracranial Hemorrhages; Isothiocyanates; Leukoencephalopathies; Lipid Metabolism; Lipid Peroxidation; Lipopolysaccharides; Liver Diseases; Lysosomes; Macrophage Colony-Stimulating Factor; Macrophages; Microglia; Microscopy; Microtubules; Mitochondria; Monocytes; Multiple Sclerosis; Mutation; Mycoses; Myelin Basic Protein; Myelin Sheath; Myeloid Cells; NF-E2-Related Factor 2; Nervous System Diseases; Nervous System Malformations; Neurites; Neurodegenerative Diseases; Neurofibrillary Tangles; Neuroinflammatory Diseases; Neurons; Neutrophils; Nucleotide Motifs; Obesity; Organelles; Organic Chemicals; Organoids; Outcome Assessment, Health Care; Oxidative Stress; Parkinson Disease; Patient Advocacy; Phagocytosis; Phenotype; Phosphorylation; Physicians; Pick Disease of the Brain; Plaque, Amyloid; Pluripotent Stem Cells; Presenilin-1; Prosencephalon; Protein Isoforms; Proteomics; Quantitative Trait Loci; RNA; Rare Diseases; Receptor, Macrophage Colony-Stimulating Factor; Receptor, Transforming Growth Factor-beta Type II; Receptors, Chimeric Antigen; Receptors, Granulocyte-Macrophage Colony-Stimulating Factor; Research Report; Resilience, Psychological; Risk Factors; Schizophrenia; Sequence Analysis, RNA; Sex Factors; Signal Transduction; Single-Cell Gene Expression Analysis; Smad2 Protein; Social Cohesion; Stem Cell Research; Stem Cells; Sulfoxides; Synaptophysin; Tauopathies; Thalamus; Tissue Distribution; Toll-Like Receptor 4; Transcription Factors; Transcriptional Activation; Transcriptome; Transforming Growth Factor beta; Transplantation, Heterologous; Treatment Outcome; Twins, Monozygotic; Weaning; White Matter; Whole Genome Sequencing; Xenon; anti-synaptophysin; heparin proteoglycan; peptide A; tau Proteins</t>
         </is>
       </c>
     </row>
@@ -605,7 +605,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Acetylation; Biological Phenomena; Blastocyst; Blastula; Cadmium; Caenorhabditis elegans; Cell Differentiation; Cell Line, Tumor; Cell Lineage; Central Nervous System; Chromatin; Computational Biology; Congenital Abnormalities; Consensus Sequence; Curriculum; DNA; DNA-Binding Proteins; Developmental Biology; Ectoderm; Embryonic Development; Embryonic Structures; Endoderm; Endodermal Sinus Tumor; Epidermis; Epigenesis, Genetic; Epigenomics; Fertilization; Fetus; Forkhead Transcription Factors; Gastrula; Gastrulation; Gene Expression; Gene Expression Profiling; Gene Expression Regulation; Gene Expression Regulation, Developmental; Gene Regulatory Networks; Genes, Developmental; Genome; Genomics; Germ Layers; HEK293 Cells; HeLa Cells; Hippo Signaling Pathway; Histone Deacetylase 1; Histone Deacetylase 2; Histone Deacetylases; Histones; Homeostasis; Inactivation, Metabolic; Lysine; Mesoderm; Multiomics; Mutation; N-Myc Proto-Oncogene Protein; Nervous System; Neural Tube; Neurulation; Nutrients; Phenotype; Phosphorylation; Pregnancy Complications; Preimplantation Diagnosis; Protein Binding; Protein Serine-Threonine Kinases; Proteomics; RNA; Regenerative Medicine; SOXB1 Transcription Factors; Sequence Analysis, RNA; Signal Transduction; Stem Cell Research; Stress, Physiological; Thinking; Transcription Factor MTF-1; Transcription Factors; Transcription, Genetic; Tumor Suppressor Proteins; Uterus; Xenopus; Xenopus Proteins; Xenopus laevis; Zinc; Zygote; animal cap</t>
+          <t>Acetylation; Biological Phenomena; Blastocyst; Blastula; Cadmium; Caenorhabditis elegans; Cell Differentiation; Cell Line, Tumor; Cell Lineage; Central Nervous System; Chromatin; Computational Biology; Congenital Abnormalities; Consensus Sequence; Curriculum; DNA; DNA-Binding Proteins; Developmental Biology; Ectoderm; Embryo, Nonmammalian; Embryonic Development; Embryonic Structures; Endoderm; Endodermal Sinus Tumor; Epidermis; Epigenesis, Genetic; Epigenomics; Fertilization; Fetus; Forkhead Transcription Factors; Gastrula; Gastrulation; Gene Expression; Gene Expression Profiling; Gene Expression Regulation; Gene Expression Regulation, Developmental; Gene Regulatory Networks; Genes, Developmental; Genome; Genomics; Germ Layers; HEK293 Cells; HeLa Cells; Hippo Signaling Pathway; Histone Deacetylase 1; Histone Deacetylase 2; Histone Deacetylases; Histones; Homeostasis; Inactivation, Metabolic; Lysine; Mesoderm; Multiomics; Mutation; N-Myc Proto-Oncogene Protein; Nervous System; Neural Tube; Neurulation; Nutrients; Phenotype; Phosphorylation; Pregnancy Complications; Preimplantation Diagnosis; Protein Binding; Protein Serine-Threonine Kinases; Proteomics; RNA; Regenerative Medicine; SOXB1 Transcription Factors; Sequence Analysis, RNA; Signal Transduction; Stem Cell Research; Stress, Physiological; Thinking; Transcription Factor MTF-1; Transcription Factors; Transcription, Genetic; Tumor Suppressor Proteins; Uterus; Xenopus; Xenopus Proteins; Xenopus laevis; Zinc; Zygote; animal cap</t>
         </is>
       </c>
     </row>
@@ -617,7 +617,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Adolescent; Alzheimer Disease; Artificial Intelligence; Brain; Cerebral Cortex; Cognition; Cognitive Neuroscience; Cognitive Science; Computer Simulation; Confusion; Depression; Diffusion Magnetic Resonance Imaging; Figural Aftereffect; Functional Neuroimaging; Gray Matter; Gyrus Cinguli; Head; Hippocampus; Individuality; Interpersonal Relations; Judgment; Learning; Magnetic Resonance Imaging; Maze Learning; Memory; Memory, Episodic; Menopause; Motion; Motion Perception; Neuroimaging; Neurons; Organ Size; Parietal Lobe; Pregnancy; Spatial Learning; Spatial Memory; Spatial Navigation; Temporal Lobe; Theta Rhythm; Virtual Reality; White Matter; Young Adult</t>
+          <t>Adolescent; Alzheimer Disease; Artificial Intelligence; Brain; Cerebral Cortex; Cognition; Cognitive Neuroscience; Cognitive Science; Computer Simulation; Confusion; Depression; Diffusion Magnetic Resonance Imaging; Exploratory Behavior; Figural Aftereffect; Functional Neuroimaging; Gray Matter; Gyrus Cinguli; Head; Hippocampus; Individuality; Interpersonal Relations; Judgment; Learning; Magnetic Resonance Imaging; Maze Learning; Memory; Memory, Episodic; Menopause; Motion; Motion Perception; Neuroimaging; Neurons; Organ Size; Parietal Lobe; Pregnancy; Sex Factors; Spatial Learning; Spatial Memory; Spatial Navigation; Temporal Lobe; Theta Rhythm; Virtual Reality; White Matter; Young Adult</t>
         </is>
       </c>
     </row>
@@ -629,7 +629,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Aging; Artificial Intelligence; Cell Line; Chromatin Immunoprecipitation; Computational Biology; DNA Damage; Databases, Factual; Generative Artificial Intelligence; Genomics; Language; Large Language Models; Liquid Biopsy; Medicine; Mutation; Neoplasms; Noninvasive Prenatal Testing; Programming Languages; Software; Systems Biology; nan</t>
+          <t>Aging; Artificial Intelligence; Cell Line; Chromatin Immunoprecipitation; Computational Biology; Consensus; DNA Damage; Databases, Factual; Generative Artificial Intelligence; Genomics; Language; Large Language Models; Liquid Biopsy; Medicine; Mutation; Neoplasms; Noninvasive Prenatal Testing; Peer Review; Programming Languages; Software; Systems Biology</t>
         </is>
       </c>
     </row>
@@ -677,7 +677,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Acoustics; Apoptosis; Astrocytes; Auditory Pathways; Axon Guidance; Axons; Biological Evolution; Brain; Brain Stem; Caspase 3; Caspases; Cell Death; Cochlear Nerve; Cysteine; Deafness; Dendrites; Embryonic Development; Endopeptidases; Evoked Potentials, Auditory, Brain Stem; Exosomes; Gene Expression Regulation; Gene Ontology; Hearing; Microglia; Myelin Sheath; Nervous System; Neurodevelopmental Disorders; Neuroglia; Neuronal Plasticity; Neurons; Oligodendroglia; Peptide Hydrolases; Phylogeny; Presynaptic Terminals; Proteomics; RNA, Long Noncoding; Synapses; Synaptic Transmission; Tandem Mass Spectrometry; Transcriptome; Trapezoid Body; nan</t>
+          <t>Acoustics; Apoptosis; Astrocytes; Auditory Pathways; Axon Guidance; Axons; Biological Evolution; Brain; Brain Stem; Caspase 3; Caspases; Cell Death; Cochlear Nerve; Cysteine; Deafness; Dendrites; Embryonic Development; Endopeptidases; Evoked Potentials, Auditory, Brain Stem; Exosomes; Gene Expression Regulation; Gene Ontology; Hearing; Microglia; Myelin Sheath; Nervous System; Neurodevelopmental Disorders; Neuroglia; Neuronal Plasticity; Neurons; Oligodendroglia; Peptide Hydrolases; Phylogeny; Presynaptic Terminals; Proteomics; RNA, Long Noncoding; Synapses; Synaptic Transmission; Tandem Mass Spectrometry; Transcriptome; Trapezoid Body</t>
         </is>
       </c>
     </row>
@@ -845,7 +845,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Acclimatization; Adaptation, Physiological; Alkaline Phosphatase; Aminopeptidases; Amylases; Animal Husbandry; Biological Evolution; Body Size; Carnivory; Cellulases; Chromosomes; Cold Temperature; Diet; Diet, Food, and Nutrition; Dietary Fiber; Digestion; Digestive System Physiological Phenomena; Ecological and Environmental Phenomena; Ecosystem; Enzymes; Esters; Fermentation; Fires; Fishes; Gastrointestinal Microbiome; Gastropoda; Gene Expression Profiling; Genetics; Genome; Genomics; Heat-Shock Response; Leucine; Lipase; Lizards; Marine Biology; Microbiota; Mytilus; Pancreatic alpha-Amylases; Perciformes; Phylogeny; Physiology; RNA, Ribosomal, 16S; Reproducibility of Results; Stomach; Temperature; Transcriptome; Trypsin; Zebrafish; alpha-Glucosidases; nan</t>
+          <t>Acclimatization; Adaptation, Physiological; Alkaline Phosphatase; Aminopeptidases; Amylases; Animal Husbandry; Bays; Biological Evolution; Body Size; California; Carbohydrates; Carboxylesterase; Carnivory; Cellulases; Chromosomes; Cold Temperature; Conservation of Natural Resources; DNA Copy Number Variations; Diet; Diet, Food, and Nutrition; Dietary Fiber; Digestion; Digestive System Physiological Phenomena; Ecological and Environmental Phenomena; Ecosystem; Endangered Species; Enzymes; Esters; Fatty Acids, Essential; Fermentation; Fires; Fisheries; Fishes; Gametogenesis; Gastrointestinal Microbiome; Gastrointestinal Tract; Gastropoda; Gene Dosage; Gene Expression Profiling; Genetics; Genome; Genomics; Heat-Shock Response; Herbivory; Hydrogen-Ion Concentration; Hydrolysis; Immunohistochemistry; Leucine; Life Cycle Stages; Lipase; Lipids; Lizards; Macrocystis; Marine Biology; Mexico; Microalgae; Microbiota; Mytilus; Pancreatic alpha-Amylases; Parents; Perciformes; Phylogeny; Physiology; Protein Isoforms; Proteomics; RNA, Ribosomal, 16S; Reproducibility of Results; Reproduction; Stomach; Temperature; Transcriptome; Trypsin; Zebrafish; alpha-Glucosidases</t>
         </is>
       </c>
     </row>
@@ -869,7 +869,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Adaptive Immunity; Aging; Algorithms; Allergy and Immunology; Alzheimer Disease; Amino Acids; Amyloid; Amyloid beta-Peptides; Amyloid beta-Protein Precursor; Amyloidogenic Proteins; Antibodies; Antibodies, Monoclonal; Antibody Specificity; Bacteriophages; Brain; Brain-Derived Neurotrophic Factor; CA1 Region, Hippocampal; Calcium; Cognition; Communicable Diseases; Congo Red; Energy Metabolism; Epitopes; Glutathione; High-Throughput Nucleotide Sequencing; Hypertension; Immunity; Immunity, Innate; Immunotherapy; Indicators and Reagents; Infant; Microglia; Neurodegenerative Diseases; Neurofibrillary Tangles; Peptides; Phosphatidylinositol-3,4,5-Trisphosphate 5-Phosphatases; Plaque, Amyloid; Pre-Eclampsia; Pregnancy; Protein Conformation, beta-Strand; Proteinuria; Serum Amyloid A Protein; Single-Domain Antibodies; Statistics, Nonparametric; Supranuclear Palsy, Progressive; Synucleins; Vaccines; Virulence; tau Proteins</t>
+          <t>Adaptive Immunity; Aging; Algorithms; Allergy and Immunology; Alzheimer Disease; Amino Acids; Amyloid; Amyloid beta-Peptides; Amyloid beta-Protein Precursor; Amyloidogenic Proteins; Antibodies; Antibodies, Monoclonal; Antibody Specificity; Autoantibodies; Bacteriophages; Brain; Brain-Derived Neurotrophic Factor; CA1 Region, Hippocampal; Calcium; Cognition; Communicable Diseases; Congo Red; Desmoglein 1; Desmoglein 3; Energy Metabolism; Epitopes; Glutathione; High-Throughput Nucleotide Sequencing; Hypertension; Immunity; Immunity, Innate; Immunotherapy; Indicators and Reagents; Infant; Keratinocytes; Microglia; Neurodegenerative Diseases; Neurofibrillary Tangles; Pemphigus; Peptides; Phosphatidylinositol-3,4,5-Trisphosphate 5-Phosphatases; Plaque, Amyloid; Pre-Eclampsia; Pregnancy; Protein Conformation, beta-Strand; Proteinuria; Receptor, Muscarinic M3; Serum Amyloid A Protein; Single-Domain Antibodies; Statistics, Nonparametric; Supranuclear Palsy, Progressive; Synucleins; Vaccines; Virulence; tau Proteins</t>
         </is>
       </c>
     </row>
@@ -881,7 +881,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Algorithms; Anti-Bacterial Agents; Bacteriophages; Biochemistry; Conotoxins; Conus Snail; Cryoelectron Microscopy; Deep Learning; Eye; Genomics; Gram-Negative Bacterial Infections; Heart; Image Processing, Computer-Assisted; Ion Channel Gating; Kinetics; Membranes; Microscopy; Models, Molecular; Molecular Structure; Multiprotein Complexes; NAV1.8 Voltage-Gated Sodium Channel; Neoplasms; Peptides; Phage Therapy; Protein Binding; Protein Conformation; Protein Folding; Proteins; Spider Venoms; Stenotrophomonas maltophilia; Voltage-Gated Sodium Channel Blockers; Wastewater</t>
+          <t>Algorithms; Anti-Bacterial Agents; Bacteriophages; Biochemistry; Brain; Conotoxins; Conus Snail; Cryoelectron Microscopy; Deep Learning; Escherichia coli; Eye; Gastrointestinal Microbiome; Genomics; Gram-Negative Bacterial Infections; Heart; Image Processing, Computer-Assisted; Ion Channel Gating; Kinetics; Membranes; Microscopy; Models, Molecular; Molecular Structure; Multiprotein Complexes; NAV1.8 Voltage-Gated Sodium Channel; Neoplasms; Peptides; Phage Therapy; Protein Conformation; Protein Folding; Proteins; Spider Venoms; Stenotrophomonas maltophilia; Virion; Voltage-Gated Sodium Channel Blockers; Wastewater; Zebrafish</t>
         </is>
       </c>
     </row>
@@ -893,7 +893,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Alanine Dehydrogenase; Anti-Bacterial Agents; Arginine; Bacteria; Bacterial Proteins; Biliverdine; Biochemistry; Bordetella pertussis; Carrier Proteins; Communicable Diseases; Cryoelectron Microscopy; Disulfides; Drug Discovery; Electrons; Enterobacter cloacae; Enzyme Inhibitors; Escherichia coli; Escherichia coli Proteins; Eukaryotic Cells; Glycation End Products, Advanced; Hemagglutinins; Heme; Heme Oxygenase (Decyclizing); Hemoglobins; Histidine Kinase; Infant; Infant, Newborn; Iron; Latent Tuberculosis; Ligands; Lysine; Mass Spectrometry; Membrane Proteins; Molecular Biology; Molecular Structure; Mycobacteriaceae; Mycobacterium tuberculosis; Nucleosides; Nutrients; Pandemics; Pertussis Vaccine; Protein Interaction Mapping; Protein Processing, Post-Translational; Protein Sorting Signals; Proteins; Proteolysis; Pyruvaldehyde; Siderophores; Tomography, X-Ray Computed; Toxins, Biological; Tuberculosis; Vaccination; Virulence; Virulence Factors; Whooping Cough; nan</t>
+          <t>Alanine Dehydrogenase; Anti-Bacterial Agents; Arginine; Bacteria; Bacterial Proteins; Biliverdine; Biochemistry; Bordetella pertussis; Carrier Proteins; Communicable Diseases; Cryoelectron Microscopy; Disulfides; Drug Discovery; Electrons; Enterobacter cloacae; Enzyme Inhibitors; Escherichia coli; Escherichia coli Proteins; Eukaryotic Cells; Glycation End Products, Advanced; Hemagglutinins; Heme; Heme Oxygenase (Decyclizing); Hemoglobins; Histidine Kinase; Infant; Infant, Newborn; Iron; Latent Tuberculosis; Ligands; Lysine; Mass Spectrometry; Membrane Proteins; Molecular Biology; Molecular Structure; Mycobacteriaceae; Mycobacterium tuberculosis; Nucleosides; Nutrients; Pandemics; Pertussis Vaccine; Protein Interaction Mapping; Protein Processing, Post-Translational; Protein Sorting Signals; Proteins; Proteolysis; Pyruvaldehyde; Siderophores; Tomography, X-Ray Computed; Toxins, Biological; Tuberculosis; Vaccination; Virulence; Virulence Factors; Whooping Cough</t>
         </is>
       </c>
     </row>
@@ -965,7 +965,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Agriculture; Anthropogenic Effects; Bacteria; Bees; Biodiversity; Biological Evolution; Coral Bleaching; Crithidia; Crops, Agricultural; DNA Contamination; Data Analysis; Disease Resistance; Dysbiosis; Ecological and Environmental Phenomena; Ecology; Ecosystem; Gastrointestinal Microbiome; Genetics; Health; Host Microbial Interactions; Human Activities; Insecta; Longevity; Magnolia; Metagenomics; Microbiota; Motivation; Parasites; Pollination; Quality Indicators, Health Care; RNA, Ribosomal, 16S; Reproduction; Schools; Seasons; Social Behavior; Social Interaction; Symbiosis</t>
+          <t>Agriculture; Anthropogenic Effects; Bacteria; Bees; Biodiversity; Biological Evolution; Coral Bleaching; Crithidia; Crops, Agricultural; DNA Contamination; Data Analysis; Diet; Disease Resistance; Dysbiosis; Ecological and Environmental Phenomena; Ecology; Ecosystem; Gastrointestinal Microbiome; Genetics; Health; Host Microbial Interactions; Human Activities; Insecta; Longevity; Magnolia; Metagenomics; Microbiota; Motivation; Parasites; Pollination; Quality Indicators, Health Care; RNA, Ribosomal, 16S; Reproduction; Schools; Seasons; Serratia marcescens; Social Behavior; Social Interaction; Symbiosis</t>
         </is>
       </c>
     </row>
@@ -989,7 +989,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Adipogenesis; Adipose Tissue; Allografts; Alzheimer Disease; Anemia; Angiogenesis; Anxiety; Apolipoprotein E2; Apolipoprotein E4; Arteries; Arteriovenous Malformations; Astrocytes; Basement Membrane; Bayes Theorem; Biomarkers, Tumor; Biomimetics; Blood Vessels; Blood-Brain Barrier; Brain; Breast; Capillaries; Cell Line, Tumor; Cell- and Tissue-Based Therapy; Clustered Regularly Interspaced Short Palindromic Repeats; Coculture Techniques; Colonic Neoplasms; Colorectal Neoplasms; Cytoreduction Surgical Procedures; Diabetes Mellitus; Drug Development; Drug Evaluation; Drug Interactions; Drug Repositioning; Endoglin; Endothelial Cells; Endothelium, Vascular; Epistaxis; Exosomes; Extracellular Matrix; Fascia; Fibroblasts; Fluorouracil; Gene Expression; Glucose; Heart Failure; Huntington Disease; Hyperthermia, Induced; Hyperthermic Intraperitoneal Chemotherapy; Immunotherapy; Immunotherapy, Adoptive; Incidence; Induced Pluripotent Stem Cells; Infant; Insulin; Islets of Langerhans; Islets of Langerhans Transplantation; Lab-On-A-Chip Devices; Leucovorin; Liver; Lung; Microfluidics; Microglia; Microphysiological Systems; Microvessels; Mutation; Myocytes, Smooth Muscle; Neoadjuvant Therapy; Neoplasms; Neoplastic Processes; Neovascularization, Pathologic; Neurons; Obesity; Oxaliplatin; Paclitaxel; Pancreas; Pancreatic Neoplasms; Patient Advocacy; Pazopanib; Peptides; Pericytes; Peritoneal Cavity; Peritoneal Neoplasms; Peritoneum; Phenotype; Port-Wine Stain; Prospective Studies; RNA; Rare Diseases; Rodentia; Signal Transduction; Single-Cell Gene Expression Analysis; Snail Family Transcription Factors; Splenic Neoplasms; Stomach Neoplasms; Stroke; Stromal Cells; Sturge-Weber Syndrome; Survival Rate; Telangiectasia, Hereditary Hemorrhagic; Thrombosis; Tight Junctions; Tissue Engineering; Transcription Factors; Transcriptome; Transcytosis; Triple Negative Breast Neoplasms; Tumor Microenvironment; Vascular Malformations; cdc42 GTP-Binding Protein; nan; peptide I; rho GTP-Binding Proteins</t>
+          <t>Adipogenesis; Adipose Tissue; Allografts; Alzheimer Disease; Anemia; Angiogenesis; Anxiety; Apolipoprotein E2; Apolipoprotein E4; Arteries; Arteriovenous Malformations; Astrocytes; Basement Membrane; Bayes Theorem; Biomarkers, Tumor; Biomimetics; Blood Substitutes; Blood Vessels; Blood-Borne Pathogens; Blood-Brain Barrier; Brain; Breast; Capillaries; Cell Line, Tumor; Central Nervous System Diseases; Clustered Regularly Interspaced Short Palindromic Repeats; Coculture Techniques; Colonic Neoplasms; Colorectal Neoplasms; Cytoreduction Surgical Procedures; Diabetes Mellitus; Drug Development; Drug Evaluation; Drug Interactions; Drug Repositioning; Endoglin; Endothelial Cells; Endothelium, Vascular; Epistaxis; Exosomes; Extracellular Matrix; Fascia; Fibroblasts; Fluorouracil; Gene Expression; Glucose; Heart Failure; Huntington Disease; Hyperthermia, Induced; Hyperthermic Intraperitoneal Chemotherapy; Incidence; Induced Pluripotent Stem Cells; Infant; Insulin; Islets of Langerhans; Islets of Langerhans Transplantation; Lab-On-A-Chip Devices; Leucovorin; Liver; Lung; Microfluidics; Microglia; Microphysiological Systems; Microvessels; Mutation; Myocytes, Smooth Muscle; Neoadjuvant Therapy; Neoplasms; Neoplastic Processes; Neovascularization, Pathologic; Neurons; Obesity; Oxaliplatin; Paclitaxel; Pancreas; Pancreatic Neoplasms; Patient Advocacy; Pazopanib; Peptides; Pericytes; Peritoneal Cavity; Peritoneal Neoplasms; Peritoneum; Phenotype; Port-Wine Stain; Prospective Studies; RNA; Rare Diseases; Rodentia; Signal Transduction; Single-Cell Gene Expression Analysis; Sitting Position; Snail Family Transcription Factors; Splenic Neoplasms; Stomach Neoplasms; Stroke; Stromal Cells; Sturge-Weber Syndrome; Survival Rate; Technology; Telangiectasia, Hereditary Hemorrhagic; Thrombosis; Tight Junctions; Tissue Engineering; Transcription Factors; Transcriptome; Transcytosis; Triple Negative Breast Neoplasms; Tumor Microenvironment; Vascular Malformations; cdc42 GTP-Binding Protein; peptide I; rho GTP-Binding Proteins</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Biodiversity; Biomass; Carbon; Climate Change; Desert Climate; Ecological and Environmental Phenomena; Ecology; Ecosystem; Fertilizers; Grassland; Groundwater; Health Surveys; Humidity; Hydrology; Museums; Nitrogen; Nutrients; Phosphorus; Physiology, Comparative; Plants; Rain; Remote Sensing Technology; Soil; Temperature; Volunteers; Water; Water Resources; Water Supply; Wind</t>
+          <t>Biodiversity; Biomass; California; Carbon; Climate Change; Desert Climate; Ecological and Environmental Phenomena; Ecology; Ecosystem; Fertilizers; Grassland; Groundwater; Health Surveys; Humidity; Hydrology; Introduced Species; Museums; Nitrogen; Nutrients; Phosphorus; Physiology, Comparative; Plants; Rain; Remote Sensing Technology; Soil; Temperature; Volunteers; Water; Water Resources; Water Supply; Wind</t>
         </is>
       </c>
     </row>
@@ -1037,7 +1037,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Adrenergic beta-Antagonists; Aged; Aged, 80 and over; Aging; Alzheimer Disease; Amyloid; Amyloid beta-Peptides; Amyloidosis; Amyotrophic Lateral Sclerosis; Angiotensin-Converting Enzyme Inhibitors; Aniline Compounds; Apolipoproteins E; Atrophy; Autopsy; Biomarkers; Brain; Case-Control Studies; Cataract; Cell Separation; Centenarians; Cerebral Cortex; Cerebrovascular Circulation; Cerebrovascular Disorders; Clinical Trials as Topic; Cognition; Cognitive Dysfunction; Cohort Studies; Cryopreservation; DNA-Binding Proteins; Databases, Factual; Dementia; Dementia, Vascular; Diagnosis, Differential; Disease Progression; Educational Status; Epidemiology; Ethnicity; Ethylene Glycols; Executive Function; Extracellular Vesicles; Frailty; Frontotemporal Lobar Degeneration; Geriatric Assessment; Hand Strength; Hippocampal Sclerosis; Hippocampus; Incidence; Inclusion Bodies; Lewy Bodies; Lewy Body Disease; Life Style; Limbic System; Logistic Models; Longitudinal Studies; Magnetic Resonance Imaging; Medical History Taking; Nervous System Diseases; Neurofibrillary Tangles; Neuroglia; Neuroimaging; Neurons; Neuropathology; Neuropsychological Tests; Nonagenarians; Organ Size; Physical Functional Performance; Plaque, Amyloid; Positron-Emission Tomography; Public Health; RNA-Seq; Racial Groups; Reference Values; Resilience, Psychological; Retrospective Studies; Risk Factors; Self Report; Self-Help Devices; Sex Factors; Sleep; Sleep Duration; Syncope; TDP-43 Proteinopathies; Tauopathies; Walking Speed; White Matter</t>
+          <t>Adrenergic beta-Antagonists; Aged; Aged, 80 and over; Aging; Alzheimer Disease; Amyloid; Amyloid beta-Peptides; Amyloidosis; Amyotrophic Lateral Sclerosis; Angiotensin-Converting Enzyme Inhibitors; Aniline Compounds; Apolipoproteins E; Atrophy; Autopsy; Biomarkers; Brain; Case-Control Studies; Cataract; Cell Separation; Centenarians; Cerebral Cortex; Cerebrovascular Circulation; Cerebrovascular Disorders; Clinical Trials as Topic; Cognition; Cognitive Dysfunction; Cohort Studies; Cryopreservation; DNA-Binding Proteins; Databases, Factual; Dementia; Dementia, Vascular; Diagnosis, Differential; Disease Progression; Educational Status; Epidemiology; Ethnicity; Ethylene Glycols; Executive Function; Extracellular Vesicles; Frailty; Frontotemporal Lobar Degeneration; Geriatric Assessment; Hand Strength; Hippocampus; Incidence; Inclusion Bodies; Lewy Bodies; Lewy Body Disease; Life Style; Limbic System; Longitudinal Studies; Magnetic Resonance Imaging; Medical History Taking; Nervous System Diseases; Neurofibrillary Tangles; Neuroglia; Neuroimaging; Neurons; Neuropsychological Tests; Nonagenarians; Organ Size; Physical Functional Performance; Plaque, Amyloid; Positron-Emission Tomography; Public Health; RNA-Seq; Racial Groups; Reference Values; Resilience, Psychological; Retrospective Studies; Risk Factors; Self Report; Self-Help Devices; Sex Factors; Sleep; Sleep Duration; Syncope; TDP-43 Proteinopathies; Tauopathies; Walking Speed; White Matter</t>
         </is>
       </c>
     </row>
@@ -1057,7 +1057,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>AMP-Activated Protein Kinases; Abdominal Cavity; Adenocarcinoma; Adenocarcinoma, Mucinous; Adenomatous Polyposis Coli; Adolescent; Allografts; Antineoplastic Agents; Appendectomy; Appendiceal Neoplasms; Ascitic Fluid; Biological Products; Cachexia; Carcinogenesis; Carcinoma; Catalytic Domain; Cell Cycle; Cell Differentiation; Cell Line; Cell Line, Tumor; Cell Plasticity; Cell Proliferation; Chemistry, Pharmaceutical; Chromatin; Chromatography, Liquid; Clinical Relevance; Colonic Neoplasms; Colorectal Neoplasms; Cost of Illness; Cytokines; Cytoreduction Surgical Procedures; DNA; Diabetes Mellitus; Diabetes Mellitus, Type 2; Diet, High-Fat; Diet, Ketogenic; Dietary Supplements; Dioxygenases; Drug Resistance, Neoplasm; Early Detection of Cancer; Epigenesis, Genetic; Epigenomics; Ficus; Gastrointestinal Neoplasms; Gene Expression; Gene Expression Regulation, Neoplastic; Genes, Tumor Suppressor; Genes, p16; Genetics; Glucose; Glutamine; Heterografts; High-Throughput Screening Assays; Histone Code; Histone Demethylases; Histone Methyltransferases; Histones; Homeostasis; Hospitalization; Hyperthermic Intraperitoneal Chemotherapy; Immunity; Immunotherapy; Incidence; Intestinal Mucosa; Isotopes; Ketoglutaric Acids; Ketone Bodies; Ketones; Lactic Acid; Lipid Metabolism; Lipids; Lipogenesis; Liquid Chromatography-Mass Spectrometry; Liver Neoplasms; Lubricants; Melanoma; Metabolic Diseases; Metabolic Networks and Pathways; Metabolism; Metformin; Micronutrients; Microscopy; Military Personnel; Monocarboxylic Acid Transporters; Morbidity; Muscles; Mutation; National Center for Advancing Translational Sciences (U.S.); Neoplasms; Neoplasms, Second Primary; Neoplastic Processes; Neoplastic Stem Cells; Nutrients; Obesity; Organoids; Ovarian Neoplasms; Oxidative Phosphorylation; PPAR gamma; Peptide Hydrolases; Peritoneal Cavity; Peritoneal Neoplasms; Peritoneum; Peroxisome Proliferator-Activated Receptors; Phenotype; Phosphoprotein Phosphatases; Phosphoric Monoester Hydrolases; Phosphorylation; Pilot Projects; Pioglitazone; Prevalence; Prostatic Neoplasms; Protein Phosphatase 2; Protein Serine-Threonine Kinases; Proteolysis; Pseudomyxoma Peritonei; Pyruvic Acid; Quality of Life; RNA; RNA, Long Noncoding; Rectal Neoplasms; Risk Factors; Sequence Analysis, RNA; Sex Characteristics; Sex Chromosomes; Signal Transduction; Standard of Care; Stem Cells; Substrate Specificity; T-Lymphocytes; TWEAK Receptor; Tandem Mass Spectrometry; Thiazolidinediones; Transcription Factors; Tumor Microenvironment; Vitamin A; Vitamin B 6; Vitamins; Weight Loss; Wnt Signaling Pathway; nan</t>
+          <t>AMP-Activated Protein Kinases; Abdominal Cavity; Adenocarcinoma; Adenocarcinoma, Mucinous; Adenomatous Polyposis Coli; Adolescent; Allografts; Antineoplastic Agents; Appendectomy; Appendiceal Neoplasms; Ascitic Fluid; Biological Products; Cachexia; Carcinogenesis; Carcinoma; Catalytic Domain; Cell Cycle; Cell Differentiation; Cell Line; Cell Line, Tumor; Cell Plasticity; Cell Proliferation; Chemistry, Pharmaceutical; Chromatin; Chromatography, Liquid; Clinical Relevance; Colonic Neoplasms; Colorectal Neoplasms; Cost of Illness; Cytokines; Cytoreduction Surgical Procedures; DNA; Diabetes Mellitus; Diabetes Mellitus, Type 2; Diet, High-Fat; Diet, Ketogenic; Dietary Supplements; Dioxygenases; Drug Resistance, Neoplasm; Early Detection of Cancer; Epigenesis, Genetic; Epigenomics; Ficus; Gastrointestinal Neoplasms; Gene Expression; Gene Expression Regulation, Neoplastic; Genes, Tumor Suppressor; Genes, p16; Genetics; Glucose; Glutamine; Heterografts; High-Throughput Screening Assays; Histone Code; Histone Demethylases; Histone Methyltransferases; Histones; Homeostasis; Hospitalization; Hyperthermic Intraperitoneal Chemotherapy; Immunity; Immunotherapy; Incidence; Intestinal Mucosa; Isotopes; Ketoglutaric Acids; Ketone Bodies; Ketones; Lactic Acid; Lipid Metabolism; Lipids; Lipogenesis; Liquid Chromatography-Mass Spectrometry; Liver Neoplasms; Lubricants; Melanoma; Metabolic Diseases; Metabolic Networks and Pathways; Metabolism; Metformin; Micronutrients; Microscopy; Military Personnel; Monocarboxylic Acid Transporters; Morbidity; Muscles; Mutation; National Center for Advancing Translational Sciences (U.S.); Neoplasms; Neoplasms, Second Primary; Neoplastic Processes; Neoplastic Stem Cells; Nutrients; Obesity; Organoids; Ovarian Neoplasms; Oxidative Phosphorylation; PPAR gamma; Peptide Hydrolases; Peritoneal Cavity; Peritoneal Neoplasms; Peritoneum; Peroxisome Proliferator-Activated Receptors; Phenotype; Phosphoprotein Phosphatases; Phosphoric Monoester Hydrolases; Phosphorylation; Pilot Projects; Pioglitazone; Prevalence; Prostatic Neoplasms; Protein Phosphatase 2; Protein Serine-Threonine Kinases; Proteolysis; Pseudomyxoma Peritonei; Pyruvic Acid; Quality of Life; RNA; RNA, Long Noncoding; Rectal Neoplasms; Risk Factors; Sequence Analysis, RNA; Sex Characteristics; Sex Chromosomes; Signal Transduction; Standard of Care; Stem Cells; Substrate Specificity; T-Lymphocytes; TWEAK Receptor; Tandem Mass Spectrometry; Thiazolidinediones; Transcription Factors; Tumor Microenvironment; Vitamin A; Vitamin B 6; Vitamins; Weight Loss; Wnt Signaling Pathway</t>
         </is>
       </c>
     </row>
@@ -1077,7 +1077,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Africa; Alleles; Animal Fins; Australia; Autism Spectrum Disorder; Autistic Disorder; Base Sequence; Brain; Brain Neoplasms; CCCTC-Binding Factor; CRISPR-Cas Systems; Cell Culture Techniques; Cell Cycle Proteins; Chromatin; Chromosomal Proteins, Non-Histone; Chromosomes; Chromosomes, Human, Pair 8; Clinical Relevance; Cohesins; Congenital Abnormalities; Craniofacial Abnormalities; DNA Transposable Elements; DNA, Intergenic; Ectopic Gene Expression; Enhancer Elements, Genetic; Epigenome; Epigenomics; Evolution, Molecular; Extinction, Biological; Extremities; Fetal Heart; Fishes; Gain of Function Mutation; Gene Expression; Gene Expression Profiling; Gene Expression Regulation; Gene Expression Regulation, Developmental; Gene Rearrangement; Genes, Reporter; Genetic Variation; Genome; Genome Size; Genomics; Glioma; Heart Diseases; Hedgehog Proteins; Homeodomain Proteins; Intellectual Disability; Introns; Isocitrate Dehydrogenase; Karyotype; Limb Buds; Locomotion; Marsupialia; MicroRNAs; Mutation; Organoids; Otx Transcription Factors; Phenotype; Phylogeny; Piwi-Interacting RNA; Polydactyly; Polymorphism, Single Nucleotide; Promoter Regions, Genetic; RNA, Long Noncoding; Regulatory Sequences, Nucleic Acid; Single-Cell Analysis; South America; Time Factors; Transcription Factors; Transcriptional Activation; Virulence; Zinc Fingers</t>
+          <t>Africa; Alleles; Animal Fins; Australia; Autism Spectrum Disorder; Autistic Disorder; Base Sequence; Binding Sites; Brain; Brain Neoplasms; CCCTC-Binding Factor; CRISPR-Cas Systems; Cell Culture Techniques; Cell Cycle Proteins; Chromatin; Chromosomal Proteins, Non-Histone; Chromosomes; Chromosomes, Human, Pair 8; Clinical Relevance; Cohesins; Congenital Abnormalities; Craniofacial Abnormalities; DNA; DNA Transposable Elements; DNA, Intergenic; Ectopic Gene Expression; Enhancer Elements, Genetic; Epigenome; Epigenomics; Evolution, Molecular; Extinction, Biological; Extremities; Fetal Heart; Fishes; Gain of Function Mutation; Gene Expression; Gene Expression Profiling; Gene Expression Regulation; Gene Expression Regulation, Developmental; Gene Rearrangement; Genes, Reporter; Genetic Code; Genetic Variation; Genome; Genome Size; Genomics; Glioma; Heart Diseases; Hedgehog Proteins; Homeodomain Proteins; Intellectual Disability; Introns; Isocitrate Dehydrogenase; Karyotype; Limb Buds; Locomotion; Marsupialia; MicroRNAs; Mutation; Nucleotide Motifs; Organoids; Otx Transcription Factors; Phenotype; Phylogeny; Piwi-Interacting RNA; Polydactyly; Polymorphism, Single Nucleotide; Promoter Regions, Genetic; Protein Binding; RNA, Long Noncoding; Regulatory Sequences, Nucleic Acid; SELEX Aptamer Technique; Single-Cell Analysis; South America; Time Factors; Transcription Factors; Transcriptional Activation; Virulence; Zinc Fingers</t>
         </is>
       </c>
     </row>
@@ -1089,7 +1089,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>ATP-Binding Cassette Transporters; Aged; Aged, 80 and over; Alzheimer Disease; Amyloid beta-Peptides; Amyloid beta-Protein Precursor; Apolipoproteins E; Asian; Astrocytes; Biomarkers; Brain; CRISPR-Associated Proteins; CRISPR-Cas Systems; Cathepsin D; Chromatin Immunoprecipitation Sequencing; Clustered Regularly Interspaced Short Palindromic Repeats; Cognition; Cuprizone; Data Management; Demyelinating Diseases; Disease Progression; Down Syndrome; Down-Regulation; Doxycycline; Endoribonucleases; Fibroblasts; Gastrointestinal Microbiome; Gene Editing; Gene Expression Profiling; Gene Expression Regulation; Gene Knock-In Techniques; Genetic Variation; Genome-Wide Association Study; Genotype; Glial Fibrillary Acidic Protein; HEK293 Cells; Hispanic or Latino; Induced Pluripotent Stem Cells; Laboratories; Leadership; Lipidomics; Longevity; Membrane Glycoproteins; Metabolome; Metabolomics; Microbiota; Microglia; Mobile Applications; Mutation; Myeloid Differentiation Factor 88; NF-kappa B; Neurodegenerative Diseases; Neuroglia; Neuroimaging; Neurons; Phagocytosis; Phenotype; Plaque, Amyloid; Proteomics; RNA Splicing; RNA-Seq; Receptors, Immunologic; Registries; Resilience, Psychological; Response Elements; Rodentia; Sex Characteristics; Signal Transduction; Single-Cell Gene Expression Analysis; Tauopathies; Tetracycline; Transcriptome; Translational Research, Biomedical; tau Proteins</t>
+          <t>ATP-Binding Cassette Transporters; Aged; Aged, 80 and over; Alzheimer Disease; Amyloid beta-Peptides; Amyloid beta-Protein Precursor; Apolipoproteins E; Asian; Astrocytes; Biomarkers; Brain; CRISPR-Associated Proteins; CRISPR-Cas Systems; Case-Control Studies; Cathepsin D; Chromatin Immunoprecipitation Sequencing; Chromosomes, Human, X; Clustered Regularly Interspaced Short Palindromic Repeats; Cognition; Cuprizone; Data Management; Demyelinating Diseases; Disease Progression; Down Syndrome; Down-Regulation; Doxycycline; Endoribonucleases; Fibroblasts; Gastrointestinal Microbiome; Gene Editing; Gene Expression Profiling; Gene Expression Regulation; Gene Knock-In Techniques; Genetic Predisposition to Disease; Genetic Variation; Genome-Wide Association Study; Genotype; Glial Fibrillary Acidic Protein; HEK293 Cells; Hispanic or Latino; Induced Pluripotent Stem Cells; Laboratories; Leadership; Lipidomics; Longevity; Membrane Glycoproteins; Metabolome; Metabolomics; Microbiota; Microglia; Mobile Applications; Mutation; Myeloid Differentiation Factor 88; NF-kappa B; Neurodegenerative Diseases; Neuroglia; Neuroimaging; Neurons; Phagocytosis; Phenotype; Plaque, Amyloid; Polymorphism, Single Nucleotide; Proteomics; RNA Splicing; RNA-Seq; Receptors, Immunologic; Registries; Resilience, Psychological; Response Elements; Rodentia; Sex Characteristics; Signal Transduction; Single-Cell Gene Expression Analysis; Tauopathies; Tetracycline; Transcriptome; Translational Research, Biomedical; X Chromosome Inactivation; tau Proteins</t>
         </is>
       </c>
     </row>
@@ -1137,7 +1137,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Aging; Anaphase-Promoting Complex-Cyclosome; CDC2 Protein Kinase; Caenorhabditis elegans; Caenorhabditis elegans Proteins; Cdc20 Proteins; Cell Cycle; Cell Cycle Checkpoints; Cell Cycle Proteins; Cell Differentiation; Cell Proliferation; Centers for Disease Control and Prevention, U.S.; Clustered Regularly Interspaced Short Palindromic Repeats; Cues; Cyclin B; Cyclin B1; Cyclin B2; Cyclins; Embryo, Nonmammalian; Embryonic Development; Ependymoglial Cells; Genomics; Germ Cells; Kinetochores; M Phase Cell Cycle Checkpoints; Microscopy; Microtubule-Associated Proteins; Mitosis; Neocortex; Neoplasms; Phosphorylation; Protein Serine-Threonine Kinases; Repressor Proteins; Spindle Apparatus; Tetratricopeptide Repeat; nan</t>
+          <t>Aging; Anaphase-Promoting Complex-Cyclosome; Antineoplastic Agents; CDC2 Protein Kinase; Caenorhabditis elegans; Caenorhabditis elegans Proteins; Cdc20 Proteins; Cell Cycle; Cell Cycle Checkpoints; Cell Cycle Proteins; Cell Differentiation; Cell Proliferation; Centers for Disease Control and Prevention, U.S.; Chromosome Segregation; Clustered Regularly Interspaced Short Palindromic Repeats; Cues; Cyclin B; Cyclin B1; Cyclin B2; Cyclins; Embryo, Nonmammalian; Embryonic Development; Ependymoglial Cells; Genomics; Germ Cells; Kinetochores; M Phase Cell Cycle Checkpoints; Microscopy; Microtubule-Associated Proteins; Mitosis; Neocortex; Neoplasms; Phosphorylation; Protein Serine-Threonine Kinases; Repressor Proteins; Spindle Apparatus; Tetratricopeptide Repeat</t>
         </is>
       </c>
     </row>
@@ -1161,7 +1161,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>AIDS Dementia Complex; Acquired Immunodeficiency Syndrome; Adaptive Immunity; Adaptor Proteins, Signal Transducing; Allergy and Immunology; Alzheimer Disease; Amyloid; Amyloid beta-Peptides; Anti-Infective Agents; Antigen Presentation; Astrocytes; Blood Coagulation; Blood-Brain Barrier; Brain; CD4-Positive T-Lymphocytes; CD8-Positive T-Lymphocytes; Capparis; Caspase 1; Caspase 8; Caspases; Cell Death; Cell Membrane; Cell Proliferation; Central Nervous System; Central Nervous System Infections; Cerebrovascular Circulation; Chemokine CCL2; Chemokines; Clustered Regularly Interspaced Short Palindromic Repeats; Coculture Techniques; Cognition; Coinfection; Communicable Disease Control; Cytokines; Dendritic Cells; Encephalitis; Endothelial Cells; Fibrin; Gasdermins; Gene Regulatory Networks; HIV Infections; Heart Transplantation; Hemodynamics; Hippo Signaling Pathway; Host-Parasite Interactions; Host-Pathogen Interactions; Immunity; Immunity, Innate; Induced Pluripotent Stem Cells; Infections; Inflammasomes; Inflammation; Inflammation Mediators; Intercellular Adhesion Molecule-1; Interleukin-1beta; Ion Channels; Lipoproteins; Liver; Macrophages; Mechanotransduction, Cellular; Memory T Cells; Metabolic Diseases; Microglia; Microscopy; Microvessels; Monocytes; Myeloid Cells; NF-kappa B; NLR Family, Pyrin Domain-Containing 3 Protein; Necroptosis; Neoplasm Recurrence, Local; Neurodegenerative Diseases; Neuroimaging; Neuroinflammatory Diseases; Neuroprotection; Neuroprotective Agents; Parasites; Perfusion; Persistent Infection; Phagocytosis; Phenotype; Plaque, Amyloid; Platelet Aggregation; Protozoan Proteins; Receptor-Interacting Protein Serine-Threonine Kinases; Receptors, Scavenger; Signal Transduction; Syk Kinase; T-Lymphocytes; T-Lymphocytes, Regulatory; THP-1 Cells; Thromboinflammation; Toxoplasma; Toxoplasmosis; Toxoplasmosis, Cerebral; Transcription Factor RelA; Virulence; Virulence Factors; nan</t>
+          <t>AIDS Dementia Complex; Acquired Immunodeficiency Syndrome; Adaptive Immunity; Adaptor Proteins, Signal Transducing; Allergy and Immunology; Alzheimer Disease; Amyloid; Amyloid beta-Peptides; Anti-Infective Agents; Antigen Presentation; Astrocytes; Blood Coagulation; Blood-Brain Barrier; Brain; CD4-Positive T-Lymphocytes; CD8-Positive T-Lymphocytes; Capparis; Caspase 1; Caspase 8; Caspases; Cell Death; Cell Membrane; Cell Proliferation; Central Nervous System; Central Nervous System Infections; Cerebrovascular Circulation; Chemokine CCL2; Chemokines; Clustered Regularly Interspaced Short Palindromic Repeats; Coculture Techniques; Cognition; Coinfection; Communicable Disease Control; Cytokines; Dendritic Cells; Encephalitis; Endothelial Cells; Fibrin; Gasdermins; Gene Regulatory Networks; HIV Infections; Heart Transplantation; Hemodynamics; Hippo Signaling Pathway; Host-Parasite Interactions; Host-Pathogen Interactions; Immunity; Immunity, Innate; Induced Pluripotent Stem Cells; Infections; Inflammasomes; Inflammation; Inflammation Mediators; Intercellular Adhesion Molecule-1; Interleukin-1beta; Ion Channels; Lipoproteins; Liver; Macrophages; Mechanotransduction, Cellular; Memory T Cells; Metabolic Diseases; Microglia; Microscopy; Microvessels; Monocytes; Myeloid Cells; NF-kappa B; NLR Family, Pyrin Domain-Containing 3 Protein; Necroptosis; Neoplasm Recurrence, Local; Neurodegenerative Diseases; Neuroimaging; Neuroinflammatory Diseases; Neuroprotection; Neuroprotective Agents; Parasites; Peptides; Perfusion; Persistent Infection; Phagocytosis; Phenotype; Plaque, Amyloid; Platelet Aggregation; Protozoan Proteins; Receptor-Interacting Protein Serine-Threonine Kinases; Receptors, Scavenger; Signal Transduction; Syk Kinase; T-Lymphocytes; T-Lymphocytes, Regulatory; THP-1 Cells; Thromboinflammation; Toxoplasma; Toxoplasmosis; Toxoplasmosis, Cerebral; Transcription Factor RelA; Virulence; Virulence Factors; tdTomato</t>
         </is>
       </c>
     </row>
@@ -1185,7 +1185,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Adaptor Proteins, Signal Transducing; Adenosine Triphosphate; Allosteric Regulation; Allosteric Site; Amines; Amino Acids; Antineoplastic Agents; Artificial Cells; Binding Sites; Biocatalysis; Biomarkers; Bioreactors; Carbohydrates; Carcinoma, Hepatocellular; Cell Line; Cell Line, Tumor; Computational Biology; Dimerization; Drug Delivery Systems; Drug Discovery; Early Detection of Cancer; Entropy; Escherichia coli; Gas Chromatography-Mass Spectrometry; Glucose 1-Dehydrogenase; Head and Neck Neoplasms; Hippo Signaling Pathway; Intrinsically Disordered Proteins; Liver Cirrhosis; Liver Neoplasms; Loss of Function Mutation; Lung Neoplasms; Models, Molecular; Molecular Dynamics Simulation; Mutation; Mutation, Missense; NAD; NADP; Neoplasms; Neurofibromin 2; Nicotinamide Mononucleotide; Normal Distribution; Nucleic Acids; Oxidation-Reduction; Oxidoreductases; Peptides; Phase Separation; Polymers; Protein Binding; Protein Biosynthesis; Protein Conformation; Protein Serine-Threonine Kinases; Protein Tyrosine Phosphatase, Non-Receptor Type 11; Proteins; Proteome; Proteomics; Pyrimidines; Signal Transduction; Solutions; Solvents; Static Electricity; Volatile Organic Compounds; Water; nan</t>
+          <t>Adaptor Proteins, Signal Transducing; Adenosine Triphosphate; Allosteric Regulation; Allosteric Site; Amines; Amino Acids; Antineoplastic Agents; Artificial Cells; Binding Sites; Biocatalysis; Biomarkers; Bioreactors; Budgets; Carbohydrates; Carcinoma, Hepatocellular; Cell Line; Cell Line, Tumor; Computational Biology; Dimerization; Drug Delivery Systems; Drug Discovery; Early Detection of Cancer; Entropy; Escherichia coli; Gas Chromatography-Mass Spectrometry; Glucose 1-Dehydrogenase; Head and Neck Neoplasms; Hippo Signaling Pathway; Intrinsically Disordered Proteins; Liver Cirrhosis; Liver Neoplasms; Loss of Function Mutation; Lung Neoplasms; Models, Molecular; Molecular Dynamics Simulation; Mutation; Mutation, Missense; NAD; NADP; Neoplasms; Neurofibromin 2; Nicotinamide Mononucleotide; Normal Distribution; Nucleic Acids; Oxidation-Reduction; Oxidoreductases; Peptides; Phase Separation; Polymers; Protein Binding; Protein Biosynthesis; Protein Conformation; Protein Serine-Threonine Kinases; Protein Tyrosine Phosphatase, Non-Receptor Type 11; Proteins; Proteome; Proteomics; Pyrimidines; Signal Transduction; Solutions; Solvents; Static Electricity; Volatile Organic Compounds</t>
         </is>
       </c>
     </row>
@@ -1197,7 +1197,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Action Potentials; Adenosine Triphosphate; Adolescent; Adverse Childhood Experiences; Aging; Amblyopia; Animal Care Committees; Brain; Calcium Channels; Central Nervous System; Cholinergic Neurons; Cognition; Decision Making; Electronic Nicotine Delivery Systems; Electrophysiology; Genetics; Habenula; Memory; Memory Consolidation; Memory, Short-Term; Movement; Neurons; Neurosciences; Nicotine; Nicotinic Agonists; Optogenetics; Parietal Lobe; Patch-Clamp Techniques; Postsynaptic Potential Summation; Primary Visual Cortex; Psychomotor Performance; Pyramidal Cells; Receptors, Purinergic P2; Rejuvenation; Reward; Software; Stress, Psychological; Synapses; Synaptic Transmission; Visual Acuity; Wakefulness; nan</t>
+          <t>Action Potentials; Adenosine Triphosphate; Adolescent; Adverse Childhood Experiences; Aging; Amblyopia; Animal Care Committees; Anticonvulsants; Basolateral Nuclear Complex; Brain; Calcium Channels; Central Nervous System; Cholinergic Neurons; Cognition; Computer Simulation; Decision Making; Electroencephalography; Electronic Nicotine Delivery Systems; Electrophysiology; Epilepsy; Epilepsy, Temporal Lobe; Genetics; Habenula; Hippocampus; Memory; Memory Consolidation; Memory, Short-Term; Mental Disorders; Movement; Neural Pathways; Neurons; Neurosciences; Nicotine; Nicotinic Agonists; Optogenetics; Parietal Lobe; Patch-Clamp Techniques; Postsynaptic Potential Summation; Primary Visual Cortex; Psychomotor Performance; Pyramidal Cells; Quality of Life; Receptors, Purinergic P2; Rejuvenation; Reward; Seizures; Software; Stress, Psychological; Synapses; Synaptic Transmission; Visual Acuity; Wakefulness</t>
         </is>
       </c>
     </row>
@@ -1233,7 +1233,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Adolescent; Adverse Childhood Experiences; Aerosols; Amphetamine; Analgesics, Opioid; Anhedonia; Arachidonic Acids; Basal Forebrain; Basolateral Nuclear Complex; Brain; Cannabidiol; Cannabis; Chromatography, High Pressure Liquid; Clozapine; Cognition; Conditioning, Operant; Corticotropin-Releasing Hormone; Designer Drugs; Dopamine; Dopaminergic Neurons; Dose-Response Relationship, Drug; Dronabinol; Endocannabinoids; Genetics; Growth and Development; Learning; Mass Spectrometry; Microsomes; Morphine; Motivation; Neural Pathways; Neurobiology; Nucleus Accumbens; Ovarian Follicle; Ovarian Reserve; Polyunsaturated Alkamides; Prefrontal Cortex; Rats, Long-Evans; Rats, Sprague-Dawley; Reward; Substance-Related Disorders; Tandem Mass Spectrometry; Vaping; Ventral Tegmental Area; gamma-Aminobutyric Acid</t>
+          <t>Adolescent; Adolescent Development; Adverse Childhood Experiences; Aerosols; Amphetamine; Analgesics, Opioid; Anhedonia; Arachidonic Acids; Basal Forebrain; Basolateral Nuclear Complex; Brain; Cannabidiol; Cannabis; Chromatography, High Pressure Liquid; Clozapine; Cognition; Conditioning, Operant; Corticotropin-Releasing Hormone; Designer Drugs; Dopamine; Dopaminergic Neurons; Dose-Response Relationship, Drug; Dronabinol; Endocannabinoids; Genetics; Growth and Development; Learning; Mass Spectrometry; Microglia; Microsomes; Morphine; Motivation; Neural Pathways; Neurobiology; Neuronal Plasticity; Nucleus Accumbens; Ovarian Follicle; Ovarian Reserve; Polyunsaturated Alkamides; Prefrontal Cortex; Rats, Long-Evans; Rats, Sprague-Dawley; Reward; Substance-Related Disorders; Tandem Mass Spectrometry; Vaping; Ventral Tegmental Area; gamma-Aminobutyric Acid</t>
         </is>
       </c>
     </row>
@@ -1245,7 +1245,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Biological Evolution; Biomechanical Phenomena; Carbon; Coral Reefs; Ecological and Environmental Phenomena; Ecosystem; Evolution, Molecular; Extinction, Biological; Feeding Behavior; Fishes; Genetic Speciation; Jaw; Mandible; Motion; Movement; Natural History; Perciformes; Phylogeny; Predatory Behavior; Somatotypes; Swimming; Water; nan</t>
+          <t>Aquatic Organisms; Biological Evolution; Biomechanical Phenomena; Carbon; Characidae; Coral Reefs; Ecological and Environmental Phenomena; Ecosystem; Evolution, Molecular; Extinction, Biological; Feeding Behavior; Fishes; Genetic Speciation; Information Services; Jaw; Mandible; Motion; Movement; Natural History; Perciformes; Phylogeny; Predatory Behavior; Schools; Social Behavior; Social Factors; Somatotypes; Swimming; Water</t>
         </is>
       </c>
     </row>
@@ -1305,7 +1305,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Allergy and Immunology; Apoptosis; Bacteria; Bacterial Infections; Bacteriophage P22; Binding Sites; CRISPR-Cas Systems; Capsid; Carcinoma, Hepatocellular; Caspase 1; Cell Culture Techniques; Cell Survival; Clostridium acetobutylicum; Cryoelectron Microscopy; Cryopyrin-Associated Periodic Syndromes; Cytokines; DNA; DNA Glycosylases; DNA, Mitochondrial; DNA, Viral; Drug Discovery; Endodeoxyribonucleases; Epithelium; Fluorocarbons; Galium; Gasdermins; Gene Editing; Heat-Shock Response; Host Microbial Interactions; Imaging, Three-Dimensional; Immune System; Inflammasomes; Inflammation; Interleukin-1; Interleukin-18; Interleukin-1beta; Ligands; Liver Neoplasms; Macromolecular Substances; Mass Spectrometry; Membrane Fluidity; Microscopy, Electron, Transmission; Mitochondria; Mitochondrial Diseases; Molecular Structure; Mutagenesis; NLR Family, Pyrin Domain-Containing 3 Protein; Neoplasms; Non-alcoholic Fatty Liver Disease; Nucleic Acids; Oxidative Stress; Oxides; Pathogen-Associated Molecular Pattern Molecules; Protein Binding; Protein Processing, Post-Translational; Protein Subunits; Proteins; Pyrin; Pyrin Domain; RNA; Signal Transduction; Signal-To-Noise Ratio; Virus Assembly; nan</t>
+          <t>Allergy and Immunology; Amino Acids; Apoptosis; Bacteria; Bacterial Infections; Bacteriophage P22; Binding Sites; CRISPR-Cas Systems; Capsid; Carcinoma, Hepatocellular; Caspase 1; Cell Culture Techniques; Cell Survival; Clostridium acetobutylicum; Cryoelectron Microscopy; Cryopyrin-Associated Periodic Syndromes; Cytokines; DNA; DNA Glycosylases; DNA, Mitochondrial; DNA, Viral; Drug Discovery; Endodeoxyribonucleases; Epithelium; Fluorocarbons; Galium; Gasdermins; Gene Editing; Heat-Shock Response; Host Microbial Interactions; Imaging, Three-Dimensional; Immune System; Immunity, Innate; Inflammasomes; Inflammation; Inflammation Mediators; Interleukin-1; Interleukin-18; Interleukin-1beta; Ligands; Liver Neoplasms; Macromolecular Substances; Macrophages; Mass Spectrometry; Membrane Fluidity; Microscopy, Electron, Transmission; Mitochondria; Mitochondrial Diseases; Molecular Structure; Mutagenesis; Mutation; NLR Family, Pyrin Domain-Containing 3 Protein; Neoplasms; Non-alcoholic Fatty Liver Disease; Nucleic Acids; Oxidative Stress; Oxides; Pathogen-Associated Molecular Pattern Molecules; Protein Binding; Protein Processing, Post-Translational; Protein Subunits; Proteins; Pyrin; Pyrin Domain; RNA; Signal Transduction; Signal-To-Noise Ratio; Virus Assembly</t>
         </is>
       </c>
     </row>
@@ -1353,7 +1353,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Amino Acid Substitution; Amino Acids; Antiparasitic Agents; Apicoplasts; Biolistics; Cells, Cultured; Chemistry, Pharmaceutical; Chlamydomonas; Clemastine; Colchicine; Communicable Diseases; Cryptosporidiosis; Cryptosporidium; Cryptosporidium parvum; Cytoskeleton; Drug Resistance; Embryophyta; Eukaryota; Fibroblasts; Genes, Essential; Germ Cells; Haploidy; Helminths; Herbicides; Histamine Antagonists; Household Work; Ligands; Macronucleus; Malaria; Meiosis; Micronucleus, Germline; Microtubules; Mitosis; Morbidity; Mutation; Mutation, Missense; Neoplasms; Paclitaxel; Parasites; Paromomycin; Pharmaceutical Preparations; Plasmids; Protozoan Proteins; Recombination, Genetic; Solubility; Tetrahymena; Toxoplasma; Transfection; Treatment Outcome; Tropism; Tubulin; Vertebrates; nan; oryzalin; pendimethalin; pironetin; pronamide</t>
+          <t>Amino Acid Substitution; Amino Acids; Antiparasitic Agents; Apicoplasts; Binding Sites; Biolistics; Cell Shape; Cells, Cultured; Chemistry, Pharmaceutical; Chlamydomonas; Clemastine; Colchicine; Communicable Diseases; Cryptosporidiosis; Cryptosporidium; Cryptosporidium parvum; Cytokinesis; Cytoskeleton; Drug Resistance; Embryophyta; Eukaryota; Fibroblasts; Genes, Essential; Germ Cells; Haploidy; Helminths; Herbicides; Histamine Antagonists; Household Work; Ligands; Macronucleus; Malaria; Meiosis; Micronucleus, Germline; Microtubules; Mitosis; Morbidity; Mutation; Mutation, Missense; Neoplasms; Paclitaxel; Parasites; Paromomycin; Pharmaceutical Preparations; Plasmids; Protozoan Proteins; Recombination, Genetic; Solubility; Tetrahymena; Toxoplasma; Transfection; Treatment Outcome; Tropism; Tubulin; Vertebrates; oryzalin; pendimethalin; pironetin; pronamide</t>
         </is>
       </c>
     </row>
@@ -1377,7 +1377,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Adaptive Immunity; Adipose Tissue; Adiposity; Aged; Aging; Allergy and Immunology; Anabolic Androgenic Steroids; Androgens; Anti-Inflammatory Agents; Antibodies; Antibodies, Neutralizing; Antibody Formation; Antigen Presentation; Antigens, CD1; Autoantibodies; Autoantigens; Autoimmune Diseases; B-Lymphocyte Subsets; Biocompatible Materials; Blood Glucose; CD8-Positive T-Lymphocytes; COVID-19; Cardiac Output; Cardiovascular Diseases; Carrier Proteins; Cell Differentiation; Cell Fractionation; Cell Line; Cell Line, Tumor; Cell Membrane; Cell Plasticity; Cell Proliferation; Cell Survival; Cellular Senescence; Coculture Techniques; Computer Simulation; Cross-Sectional Studies; Culture Media, Conditioned; Cytokines; Diabetes Mellitus; Diabetes Mellitus, Type 2; Diet; Diet, High-Fat; Disease Progression; Drug Evaluation, Preclinical; Endocrinology; Ethnic and Racial Minorities; Fertility; Flow Cytometry; Follicle Stimulating Hormone; Gene Expression Profiling; Gene Expression Regulation, Neoplastic; Glucose; Glucose Transporter Type 1; Glycated Hemoglobin; Glycolysis; Gonadal Steroid Hormones; Gonadotropins; Gonadotropins, Pituitary; H3B-8800; Homeostasis; Immunophenotyping; Immunotherapy; Industrial Development; Infertility; Inflammation; Inflammation Mediators; Influenza Vaccines; Insulin; Insulin Resistance; Interleukin-17; Laboratories; Lipid Metabolism; Lipids; Lipopolysaccharides; Losartan; Luteinizing Hormone; Lymphocytic Choriomeningitis; Lymphocytic choriomeningitis virus; Lymphoid Tissue; Memory B Cells; Metabolic Networks and Pathways; Metabolism; Methanol; Mexican Americans; Mice, Obese; Neoplastic Stem Cells; Obesity; Organoids; Ovarian Neoplasms; Palatine Tonsil; Pandemics; Persistent Infection; Phenotype; Pituitary Diseases; Pituitary Gland; Polycystic Ovary Syndrome; Preceptorship; Prevalence; Printing, Three-Dimensional; Professional Competence; Proprotein Convertase 9; Protein Array Analysis; Protein Transport; Proteins; Proto-Oncogene Proteins c-akt; Quality of Life; RNA, Long Noncoding; Reproduction; Research Personnel; Risk Factors; Sedentary Behavior; Sequence Analysis, RNA; Signal Transduction; Single-Cell Gene Expression Analysis; Solvents; T-Lymphocytes; Technology; Testosterone; Th17 Cells; Transcriptome; Up-Regulation; Weight Loss; Workflow; lobeglitazone; polyvinylidene fluoride</t>
+          <t>Adaptive Immunity; Adipose Tissue; Adiposity; Aged; Aging; Allergy and Immunology; Anabolic Androgenic Steroids; Androgens; Anti-Inflammatory Agents; Antibodies; Antibodies, Neutralizing; Antibody Formation; Antigen Presentation; Antigens, CD1; Autoantibodies; Autoantigens; Autoimmune Diseases; B-Lymphocyte Subsets; Bacteriophages; Biocompatible Materials; Blood Glucose; Brain; CD8-Positive T-Lymphocytes; COVID-19; Cardiac Output; Cardiovascular Diseases; Carrier Proteins; Cell Differentiation; Cell Fractionation; Cell Line; Cell Line, Tumor; Cell Membrane; Cell Plasticity; Cell Proliferation; Cell Survival; Cellular Senescence; Coculture Techniques; Computer Simulation; Cross-Sectional Studies; Culture Media, Conditioned; Cytokines; Diabetes Mellitus; Diabetes Mellitus, Type 2; Diet; Diet, High-Fat; Disease Progression; Drug Evaluation, Preclinical; Endocrinology; Escherichia coli; Ethnic and Racial Minorities; Fertility; Flow Cytometry; Follicle Stimulating Hormone; Gastrointestinal Microbiome; Gene Expression Profiling; Gene Expression Regulation, Neoplastic; Glucose; Glucose Transporter Type 1; Glycated Hemoglobin; Glycolysis; Gonadal Steroid Hormones; Gonadotropins; Gonadotropins, Pituitary; H3B-8800; Homeostasis; Immunophenotyping; Immunotherapy; Industrial Development; Infertility; Inflammation; Inflammation Mediators; Influenza Vaccines; Insulin; Insulin Resistance; Interleukin-17; Laboratories; Lipid Metabolism; Lipids; Lipopolysaccharides; Losartan; Luteinizing Hormone; Lymphocytic Choriomeningitis; Lymphocytic choriomeningitis virus; Lymphoid Tissue; Memory B Cells; Metabolic Networks and Pathways; Metabolism; Methanol; Mexican Americans; Mice, Obese; Neoplastic Stem Cells; Obesity; Organoids; Ovarian Neoplasms; Palatine Tonsil; Pandemics; Persistent Infection; Phenotype; Pituitary Diseases; Pituitary Gland; Polycystic Ovary Syndrome; Preceptorship; Prevalence; Printing, Three-Dimensional; Professional Competence; Proprotein Convertase 9; Protein Array Analysis; Protein Transport; Proteins; Proto-Oncogene Proteins c-akt; Quality of Life; RNA, Long Noncoding; Reproduction; Research Personnel; Risk Factors; Sedentary Behavior; Sequence Analysis, RNA; Signal Transduction; Single-Cell Gene Expression Analysis; Solvents; T-Lymphocytes; Technology; Testosterone; Th17 Cells; Transcriptome; Up-Regulation; Virion; Weight Loss; Workflow; Zebrafish; lobeglitazone; polyvinylidene fluoride</t>
         </is>
       </c>
     </row>
@@ -1389,7 +1389,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Adenosine; Adipocytes; Adjuvants, Immunologic; Algorithms; Alpha-Ketoglutarate-Dependent Dioxygenase FTO; Alzheimer Disease; Amyotrophic Lateral Sclerosis; Antibodies, Neutralizing; Antibodies, Viral; Benchmarking; Big Data; Biocompatible Materials; Biological Phenomena; Biomechanical Phenomena; CD8-Positive T-Lymphocytes; COVID-19; Cardiomyopathy, Dilated; Cartilage; Cell Body; Cell Communication; Cell Differentiation; Cell Line, Tumor; Cell Lineage; Cicatrix; Cluster Analysis; Computational Biology; Computer Simulation; Connectome; Cross-Linking Reagents; Data Analysis; Deep Learning; Developmental Biology; Down-Regulation; Drug Repositioning; Embryo, Mammalian; Embryonic Development; Endocrine System Diseases; Extracellular Fluid; Extracellular Matrix; Extracellular Space; Fibroblasts; Gelatin; Gene Expression; Gene Expression Profiling; Gene Expression Regulation; Gene Regulatory Networks; Genomics; Haploinsufficiency; Hemagglutinin Glycoproteins, Influenza Virus; Homeostasis; Hydrogels; Immune Checkpoint Inhibitors; Immunotherapy; Induced Pluripotent Stem Cells; Inducible T-Cell Co-Stimulator Protein; Inflammation; Influenza A Virus, H5N1 Subtype; Influenza Vaccines; Interleukin-2; Islets of Langerhans; Keratinocytes; Kidney Diseases; Lamin Type A; Ligands; Lipid A; Lipid Droplets; Lipid Metabolism; Lipogenesis; Lymphocytes; Macrophages; Melanoma; Melanoma, Experimental; Methylation; Methyltransferases; Mice, Inbred BALB C; Motor Neurons; Multiomics; Mutation; Myocytes, Cardiac; Nervous System Diseases; Neurons; Neurotransmitter Agents; Obesity; Oligodeoxyribonucleotides; Orthomyxoviridae Infections; Pericardium; Polysorbates; Programmed Cell Death 1 Receptor; Proteins; RANK Ligand; RNA; RNA-Seq; Rosacea; SARS-CoV-2; Saponins; Schwann Cells; Sequence Analysis, RNA; Signal Transduction; Single-Cell Analysis; Single-Cell Gene Expression Analysis; Skin; Software; Squalene; Systems Biology; T-Lymphocytes; T-Lymphocytes, Regulatory; Transcriptome; Vacuoles; Wound Healing; Young Adult; nan</t>
+          <t>Adenosine; Adipocytes; Adjuvants, Immunologic; Algorithms; Alpha-Ketoglutarate-Dependent Dioxygenase FTO; Alzheimer Disease; Amyotrophic Lateral Sclerosis; Antibodies, Neutralizing; Antibodies, Viral; Benchmarking; Big Data; Biocompatible Materials; Biological Phenomena; Biomechanical Phenomena; CD8-Positive T-Lymphocytes; COVID-19; Cardiomyopathy, Dilated; Cartilage; Cell Body; Cell Communication; Cell Cycle Checkpoints; Cell Differentiation; Cell Line, Tumor; Cell Lineage; Cellular Senescence; Chemokines; Cicatrix; Clinical Relevance; Cluster Analysis; Computational Biology; Computer Simulation; Connectome; Cross-Linking Reagents; Cues; Cytokines; Data Analysis; Deep Learning; Developmental Biology; Down-Regulation; Drug Repositioning; Embryo, Mammalian; Embryonic Development; Endocrine System Diseases; Endopeptidases; Extracellular Fluid; Extracellular Matrix; Extracellular Space; Fibroblasts; Gelatin; Gene Expression; Gene Expression Profiling; Gene Expression Regulation; Gene Regulatory Networks; Genomics; Haploinsufficiency; Hemagglutinin Glycoproteins, Influenza Virus; Homeostasis; Hydrogels; Immune Checkpoint Inhibitors; Immunotherapy; Induced Pluripotent Stem Cells; Inducible T-Cell Co-Stimulator Protein; Inflammation; Influenza A Virus, H5N1 Subtype; Influenza Vaccines; Interleukin-2; Islets of Langerhans; Keratinocytes; Kidney Diseases; Lamin Type A; Ligands; Lipid A; Lipid Droplets; Lipid Metabolism; Lipogenesis; Lymphocytes; Machine Learning; Macrophages; Melanoma; Melanoma, Experimental; Methylation; Methyltransferases; Mice, Inbred BALB C; Motor Neurons; Multiomics; Mutation; Myocytes, Cardiac; Nervous System Diseases; Neural Networks, Computer; Neurons; Neurotransmitter Agents; Obesity; Oligodeoxyribonucleotides; Orthomyxoviridae Infections; Peptide Hydrolases; Pericardium; Polysorbates; Programmed Cell Death 1 Receptor; Proteins; RANK Ligand; RNA; RNA-Seq; Rosacea; SARS-CoV-2; Saponins; Schwann Cells; Secretome; Senescence-Associated Secretory Phenotype; Sequence Analysis, RNA; Signal Transduction; Single-Cell Analysis; Single-Cell Gene Expression Analysis; Skin; Software; Squalene; Systems Biology; T-Lymphocytes; T-Lymphocytes, Regulatory; Transcriptome; Vacuoles; Wound Healing; Young Adult</t>
         </is>
       </c>
     </row>
@@ -1421,7 +1421,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Adaptor Proteins, Signal Transducing; Adipocytes; Aged; Aging; Ambystoma mexicanum; Amputation, Surgical; Biocompatible Materials; Biological Evolution; Biomechanical Phenomena; Birds; Black or African American; Body Patterning; Brazil; Calcitonin Gene-Related Peptide; Cartilage; Casein Kinase 1 epsilon; Cell Communication; Cell Line, Tumor; Cell Proliferation; Cellular Senescence; China; Chromatin; Cicatrix; Circadian Clocks; Circadian Rhythm; Collagen; Colorectal Neoplasms; Computational Biology; Computer Simulation; Cross-Linking Reagents; Culicidae; Cytokines; Cytosol; DNA, Ancient; DNA-Binding Proteins; Dengue; Dermis; Disease Progression; Disease Susceptibility; Elephants; Embryonic Development; Epidermis; Epigenesis, Genetic; Epigenomics; Epithelial Cells; Ethnicity; Evidence Gaps; Evolution, Molecular; Extracellular Matrix; Fibroblasts; Fibrosis; Flavivirus; Fossils; Gelatin; Gene Expression; Gene Expression Profiling; Gene Expression Regulation, Developmental; Gene Expression Regulation, Neoplastic; Gene Regulatory Networks; Genome; Genomics; Glycolysis; HCT116 Cells; Hair; Hair Follicle; Hispanic or Latino; Homeodomain Proteins; Homeostasis; Hydrogels; Inflammation; Inflammatory Bowel Diseases; Internship and Residency; Intestinal Mucosa; Keloid; Keratinocytes; Latin America; Lipid Droplets; Lipid Metabolism; Lipogenesis; Locomotion; Macrophages; Mammoths; Marsupialia; Mechanistic Target of Rapamycin Complex 2; Melanocytes; Mesenchymal Stem Cells; Mitochondria; Mitochondrial Proteins; Mosquito Vectors; Multifactorial Inheritance; Multiomics; Myofibroblasts; NAD; Necroptosis; Neoplasms; Nevus; Nociceptors; Obesity; Organoids; Osteopontin; Ovosiston; Pain; Pandemic Preparedness; Pandemics; Phenotype; Phosphofructokinase-2; Phosphoprotein Phosphatases; Phosphorylation; Phylogeny; Pigmentation Disorders; Protein Serine-Threonine Kinases; Proto-Oncogene Proteins c-akt; Pruritus; Public Health; R-Loop Structures; RANK Ligand; RNA; RNA, Small Interfering; Reactive Oxygen Species; Referral and Consultation; Regeneration; Regulatory Sequences, Nucleic Acid; Reptiles; Saliva; Scalp; Schools; Secretome; Senescence-Associated Secretory Phenotype; Senotherapeutics; Sequence Analysis, RNA; Serine-Threonine Kinase 3; Signal Transduction; Single-Cell Analysis; Single-Cell Gene Expression Analysis; Sirolimus; Skin; Skin Aging; Skin Diseases; Skin Physiological Phenomena; Skin Pigmentation; Software; Stem Cells; TOR Serine-Threonine Kinases; TRPV Cation Channels; Transcription Factors; Transcriptome; Tumor Suppressor Proteins; Urodela; Vaccines; Vaccinology; Vacuoles; West Nile virus; Wnt Signaling Pathway; World Health Organization; Wound Healing; X Chromosome; YAP-Signaling Proteins; Yellow Fever; Young Adult; Zebrafish; Zika Virus; Zika Virus Infection; nan</t>
+          <t>Adaptor Proteins, Signal Transducing; Adipocytes; Aged; Aging; Ambystoma mexicanum; Amputation, Surgical; Anti-Infective Agents; Autopsy; Biocompatible Materials; Biological Evolution; Biomechanical Phenomena; Birds; Black or African American; Body Patterning; Brazil; Cadaver; Calcitonin Gene-Related Peptide; Cartilage; Casein Kinase 1 epsilon; Cell Communication; Cell Line, Tumor; Cell Proliferation; Cellular Senescence; China; Chromatin; Cicatrix; Circadian Clocks; Circadian Rhythm; Collagen; Colorectal Neoplasms; Computational Biology; Computer Simulation; Cross-Linking Reagents; Culicidae; Cytokines; Cytosol; DNA, Ancient; DNA-Binding Proteins; Dengue; Dermis; Disease Progression; Disease Susceptibility; Elephants; Embryonic Development; Epidermis; Epigenesis, Genetic; Epigenomics; Epithelial Cells; Ethnicity; Evidence Gaps; Evolution, Molecular; Extracellular Matrix; Eyebrows; Eyelids; Fibroblasts; Fibrosis; Flavivirus; Fossils; Gelatin; Gene Expression; Gene Expression Profiling; Gene Expression Regulation, Developmental; Gene Expression Regulation, Neoplastic; Gene Ontology; Gene Regulatory Networks; Genome; Genome, Human; Genomics; Glycolysis; HCT116 Cells; Hair; Hair Follicle; Heterografts; Hispanic or Latino; Homeodomain Proteins; Homeostasis; Hydrogels; Inflammation; Inflammatory Bowel Diseases; Internship and Residency; Intestinal Mucosa; Keloid; Keratinocytes; Latin America; Lipid Droplets; Lipid Metabolism; Lipogenesis; Locomotion; Macrophages; Mammoths; Marsupialia; Mechanistic Target of Rapamycin Complex 2; Melanocytes; Mesenchymal Stem Cells; Mitochondria; Mitochondrial Proteins; Mosquito Vectors; Multifactorial Inheritance; Multiomics; Myofibroblasts; NAD; Necroptosis; Neoplasms; Nevus; Nociceptors; Obesity; Organoids; Osteopontin; Ovosiston; Pain; Pandemic Preparedness; Pandemics; Phenotype; Phosphofructokinase-2; Phosphoprotein Phosphatases; Phosphorylation; Phylogeny; Pigmentation Disorders; Protein Serine-Threonine Kinases; Proto-Oncogene Proteins c-akt; Pruritus; Public Health; Quality Control; R-Loop Structures; RANK Ligand; RNA; RNA, Small Interfering; RNA-Seq; Reactive Oxygen Species; Referral and Consultation; Regeneration; Regulatory Sequences, Nucleic Acid; Reptiles; Saliva; Scalp; Schools; Secretome; Senescence-Associated Secretory Phenotype; Senotherapeutics; Sequence Analysis, RNA; Serine-Threonine Kinase 3; Signal Transduction; Single-Cell Analysis; Single-Cell Gene Expression Analysis; Sirolimus; Skin; Skin Aging; Skin Diseases; Skin Physiological Phenomena; Skin Pigmentation; Software; Stem Cells; TOR Serine-Threonine Kinases; TRPV Cation Channels; Transcription Factors; Transcriptome; Tumor Suppressor Proteins; Urodela; Vaccines; Vaccinology; Vacuoles; West Nile virus; Wnt Signaling Pathway; World Health Organization; Wound Healing; X Chromosome; YAP-Signaling Proteins; Yellow Fever; Young Adult; Zebrafish; Zika Virus; Zika Virus Infection</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,11 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Algorithms; Ammonia; Arabidopsis; Awards and Prizes; Bacteria; Biological Evolution; Bioprinting; Cell Survival; Communicable Diseases; Denitrification; Droughts; Drug Resistance, Microbial; Ecological and Environmental Phenomena; Ecosystem; Evolution, Molecular; Farmers; Gases; Genetics, Population; Metabolism; Mexico; Microbiota; Natural Science Disciplines; Nitrogen; Nitrogen Cycle; Pandemics; Plants; Plasmids; Printing, Three-Dimensional; Soil; Switzerland; Synthetic Biology; Technology; United Kingdom; Water; nan</t>
+          <t>Agave; Agriculture; Algorithms; Ammonia; Arabidopsis; Awards and Prizes; Bacteria; Biological Evolution; Bioprinting; Carbon; Cell Survival; Communicable Diseases; Crops, Agricultural; Denitrification; Droughts; Drug Resistance, Microbial; Ecological and Environmental Phenomena; Ecosystem; Edible Grain; Evolution, Molecular; Farmers; Feedback
+ DNA, Single-Stranded
+ Learning
+ Ecology
+ Empirical Research; Gases; Genetics, Population; Metabolism; Mexico; Microbiota; Natural Science Disciplines; Nitrogen; Nitrogen Cycle; Pandemics; Plants; Plasmids; Printing, Three-Dimensional; Soil; Sorghum; Switzerland; Synthetic Biology; Technology; United Kingdom; Water</t>
         </is>
       </c>
     </row>
@@ -1493,7 +1497,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Academia; Algorithms; Arousal; Behavior Control; Brain; Cognition; Cognitive Dysfunction; Cognitive Neuroscience; Consciousness; Cues; Decision Making; Depression; Electroencephalography; Electrophysiology; Healthy Volunteers; Latent Infection; Leadership; Learning; Machine Learning; Magnetic Resonance Imaging; Memory; Memory Consolidation; Memory, Episodic; Mental Health; Mood Disorders; Neurobiology; Neuroimaging; Odorants; Pilot Projects; Probability; Rodentia; Sleep; Spatial Memory; Spatial Navigation; Stress Disorders, Post-Traumatic; Vacuum; Wakefulness</t>
+          <t>Academia; Algorithms; Arousal; Behavior Control; Brain; Cognition; Cognitive Dysfunction; Cognitive Neuroscience; Computational Biology; Consciousness; Cues; Data Collection; Decision Making; Depression; Electroencephalography; Electrophysiology; Healthy Volunteers; Latent Infection; Leadership; Learning; Machine Learning; Magnetic Resonance Imaging; Memory; Memory Consolidation; Memory, Episodic; Mental Health; Mood Disorders; Neurobiology; Neuroimaging; Odorants; Pilot Projects; Probability; Research Personnel; Rodentia; Sexual and Gender Minorities; Sleep; Spatial Memory; Spatial Navigation; Stress Disorders, Post-Traumatic; Vacuum; Wakefulness</t>
         </is>
       </c>
     </row>
@@ -1505,7 +1509,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Adipocytes; Animals, Genetically Modified; Aquaporins; Biological Evolution; Biomechanical Phenomena; Bone and Bones; Branchial Region; Calcium; Cartilage; Cell Cycle Proteins; Cell Lineage; Cell Polarity; Cell Proliferation; Chondrocytes; Chromosomal Proteins, Non-Histone; Cichlids; Clinical Relevance; Cohesins; Congenital Abnormalities; Craniofacial Abnormalities; Embryo, Nonmammalian; Embryology; Embryonic Development; Embryonic Induction; Extracellular Matrix; Eye Proteins; Fibroblasts; Gene Dosage; Gene Expression Profiling; Gene Expression Regulation, Developmental; Germ Cells; Gonads; Growth Plate; Hand-Foot Syndrome; Jaw; Laboratories; Lakes; Larva; Lens, Crystalline; Ligaments; Lipid Droplets; Lipid Metabolism; Lipogenesis; Malawi; Mechanotransduction, Cellular; Mesoderm; Morphogenesis; Muscle Contraction; Mutation; Obesity; Permeability; Phenotype; Quantitative Trait Loci; Receptor Tyrosine Kinase-like Orphan Receptors; Receptors, Retinoic Acid; Receptors, Wnt; Regulatory Sequences, Nucleic Acid; Sex Determination Processes; Signal Transduction; Skeleton; Skull; Species Specificity; Systems Biology; Tendons; Tenocytes; Transcription Factors; Transcriptome; Tretinoin; Vacuoles; Van Maldergem Wetzburger Verloes syndrome; Vertebrates; Water; Wnt Proteins; Wnt Signaling Pathway; Zebrafish; Zebrafish Proteins; nan</t>
+          <t>Adipocytes; Animals, Genetically Modified; Aquaporins; Biological Evolution; Biomechanical Phenomena; Bone and Bones; Branchial Region; Calcium; Cartilage; Cell Adhesion; Cell Cycle Proteins; Cell Lineage; Cell Movement; Cell Polarity; Cell Proliferation; Chondrocytes; Chromosomal Proteins, Non-Histone; Cichlids; Clinical Relevance; Cohesins; Computer Simulation; Congenital Abnormalities; Craniofacial Abnormalities; Embryo, Nonmammalian; Embryology; Embryonic Development; Embryonic Induction; Extracellular Matrix; Eye Proteins; Fibroblasts; Gene Dosage; Gene Expression; Gene Expression Profiling; Gene Expression Regulation, Developmental; Germ Cells; Gonads; Growth Plate; Hand-Foot Syndrome; Jaw; Laboratories; Lakes; Larva; Lens, Crystalline; Ligaments; Lipid Droplets; Lipid Metabolism; Lipogenesis; Malawi; Mechanotransduction, Cellular; Mesoderm; Morphogenesis; Muscle Contraction; Mutation; Neural Crest; Obesity; Permeability; Phenotype; Quantitative Trait Loci; Receptor Tyrosine Kinase-like Orphan Receptors; Receptors, Retinoic Acid; Receptors, Wnt; Regulatory Sequences, Nucleic Acid; Sex Determination Processes; Signal Transduction; Skeleton; Skull; Species Specificity; Systems Biology; Tendons; Tenocytes; Transcription Factors; Transcriptome; Tretinoin; Vacuoles; Van Maldergem Wetzburger Verloes syndrome; Vertebrates; Water; Wnt Proteins; Wnt Signaling Pathway; Zebrafish; Zebrafish Proteins</t>
         </is>
       </c>
     </row>
@@ -1577,7 +1581,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Acetylation; Adolescent; Allosteric Regulation; Animals, Genetically Modified; Brain; CA1 Region, Hippocampal; Cause of Death; Cognition; Cognitive Dysfunction; Epigenesis, Genetic; Hippocampus; Histones; Interneurons; Long-Term Potentiation; Longevity; Mortality, Premature; Mutation; N-Methylaspartate; Neuregulin-1; Nicotiana; Nicotine; Nicotinic Agonists; Phosphorylation; Prefrontal Cortex; Pregnancy; Pyramidal Cells; Quinolines; Rats, Sprague-Dawley; Receptor, Muscarinic M1; Receptors, N-Methyl-D-Aspartate; Receptors, Nicotinic; Reward; Schizophrenia; Signal Transduction; Smoking; Smoking Cessation; Tobacco Smoking; Tobacco Use; Tobacco Use Disorder; Transcription, Genetic; Tyrosine; Up-Regulation; nan; src-Family Kinases</t>
+          <t>Acetylation; Adolescent; Allosteric Regulation; Alzheimer Disease; Animals, Genetically Modified; Behavior Rating Scale; Brain; CA1 Region, Hippocampal; Cause of Death; Chemokines; Child; Cholinergic Neurons; Cognition; Cognitive Dysfunction; Cytokines; Down-Regulation; Electrophysiology; Epigenesis, Genetic; Fluorescent Antibody Technique; Hippocampus; Histone Deacetylase Inhibitors; Histone Deacetylases; Histones; Homeostasis; Interneurons; Ligands; Long-Term Potentiation; Longevity; Memory Disorders; Microglia; Mortality, Premature; Mutation; N-Methylaspartate; Neocortex; Neuregulin-1; Nicotiana; Nicotine; Nicotinic Agonists; Phosphorylation; Plaque, Amyloid; Prefrontal Cortex; Pregnancy; Pyramidal Cells; Quinolines; RNA, Messenger; Rats, Sprague-Dawley; Receptor, Muscarinic M1; Receptors, N-Methyl-D-Aspartate; Receptors, Nicotinic; Reward; Schizophrenia; Signal Transduction; Smoking; Smoking Cessation; Somatostatin; Substance-Related Disorders; Tobacco Smoking; Tobacco Use; Tobacco Use Disorder; Transcription, Genetic; Tyrosine; Up-Regulation; src-Family Kinases</t>
         </is>
       </c>
     </row>
@@ -1601,7 +1605,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Aged; Aged, 80 and over; Aging; Alzheimer Disease; Amyloid beta-Peptides; Apolipoproteins E; Astrocytes; Autism Spectrum Disorder; Axons; Brain; CD8-Positive T-Lymphocytes; Cell Communication; Cell Line; Cell Nucleus; Cell Proliferation; Cellular Reprogramming; Central Nervous System; Chromatin Immunoprecipitation Sequencing; Cocaine; Demyelinating Diseases; Disease Progression; Down Syndrome; Encephalitis Virus, Japanese; Encephalitis, Japanese; Epigenesis, Genetic; Epigenomics; Fatty Acids, Volatile; Ganglia, Spinal; Gene Expression; Gene Expression Profiling; Gene Expression Regulation; Gene Regulatory Networks; Genetic Variation; Genetics; Genomics; Habenula; Immunity, Innate; Inflammation; Integrases; Integrins; Killer Cells, Natural; Memory; MicroRNAs; Microglia; Multiomics; Multiple Sclerosis; Myelin Sheath; Myeloid Cells; NF-KappaB Inhibitor alpha; NF-kappa B; Natural Killer T-Cells; Nerve Regeneration; Nervous System Malformations; Neurodegenerative Diseases; Neuroglia; Neuroinflammatory Diseases; Neurons; Occipital Lobe; Oligodendrocyte Precursor Cells; Oligodendroglia; Parkinson Disease; Parkinsonian Disorders; Plaque, Amyloid; Postmortem Changes; Proteomics; Pseudogenes; RNA; RNA, Small Nuclear; RNA-Seq; Rats, Sprague-Dawley; Recurrence; Remyelination; Resilience, Psychological; Sensory Receptor Cells; Sequence Analysis, RNA; Signal Transduction; Single-Cell Analysis; Spatial Memory; Spinal Cord; Spinal Cord Injuries; Sterol Regulatory Element Binding Protein 1; Stroke; Substance-Related Disorders; Systems Biology; Tauopathies; Time Factors; Transcription Factors; Transcriptome; White Matter; Wound Healing; nan; tau Proteins</t>
+          <t>Aged; Aged, 80 and over; Aging; Alzheimer Disease; Amyloid beta-Peptides; Apolipoproteins E; Astrocytes; Autism Spectrum Disorder; Brain; CD8-Positive T-Lymphocytes; Cell Communication; Cell Line; Cell Nucleus; Cell Proliferation; Cellular Reprogramming; Central Nervous System; Chromatin Immunoprecipitation Sequencing; Cocaine; Cognition; Critical Pathways; Demyelinating Diseases; Disease Progression; Down Syndrome; Encephalitis Virus, Japanese; Encephalitis, Japanese; Epigenesis, Genetic; Epigenomics; Fatty Acids, Volatile; Gene Expression; Gene Expression Profiling; Gene Expression Regulation; Gene Regulatory Networks; Genes; Genetic Variation; Genetics; Genomics; Habenula; Healthy Aging; Immunity, Innate; Inflammation; Integrases; Killer Cells, Natural; Longevity; Memory; MicroRNAs; Microglia; Multiomics; Multiple Sclerosis; Myelin Sheath; Myeloid Cells; NF-KappaB Inhibitor alpha; NF-kappa B; Natural Killer T-Cells; Nervous System Malformations; Neurodegenerative Diseases; Neuroglia; Neuroinflammatory Diseases; Neurons; Occipital Lobe; Oligodendrocyte Precursor Cells; Oligodendroglia; Parkinson Disease; Parkinsonian Disorders; Plaque, Amyloid; Postmortem Changes; Prefrontal Cortex; Proteomics; Pseudogenes; Quality Control; RNA; RNA, Small Nuclear; RNA-Seq; Recurrence; Regulator; Remyelination; Reproducibility of Results; Resilience, Psychological; Risk Factors; Sequence Analysis, RNA; Signal Transduction; Single-Cell Analysis; Spatial Memory; Spinal Cord; Spinal Cord Injuries; Sterol Regulatory Element Binding Protein 1; Stroke; Substance-Related Disorders; Systems Biology; Tauopathies; Time Factors; Transcription Factors; Transcriptome; White Matter; Wound Healing; tau Proteins</t>
         </is>
       </c>
     </row>
@@ -1649,7 +1653,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>6-methyladenine; Academia; Adenosine; Aged; Algorithms; Alternative Splicing; Alzheimer Disease; Amyotrophic Lateral Sclerosis; Animals, Genetically Modified; Artificial Intelligence; Astrocytes; Ataxin-1; Atrophy; Autophagy; Biological Phenomena; Biomarkers; Biomedical Research; Biotin; Brain; Brain-Derived Neurotrophic Factor; C9orf72 Protein; Calcium Signaling; Caregivers; Case-Control Studies; Cell Death; Cell Differentiation; Cell Line; Cell- and Tissue-Based Therapy; Cells, Cultured; Cerebellum; Cerebral Cortex; Child; Child, Preschool; Chorea; Chromatin; Chromatin Immunoprecipitation Sequencing; Chromatography, Liquid; Clinical Trials, Phase I as Topic; Clustered Regularly Interspaced Short Palindromic Repeats; Cognition; Cognitive Dysfunction; Communication; Corpus Striatum; DNA Breaks, Double-Stranded; DNA Damage; DNA Repair; DNA-Binding Proteins; Deep Learning; Delayed Diagnosis; Dementia; Demography; Depression; Dihydroxyphenylalanine; Disease Progression; Dopaminergic Neurons; Drug Development; Dystonia 3, Torsion, X-Linked; Edema; Electrophysiology; Embryonic Stem Cells; Epigenesis, Genetic; Epigenomics; Epilepsies, Partial; Exons; Feasibility Studies; Fibroblasts; Frontotemporal Dementia; Frontotemporal Lobar Degeneration; Gene Editing; Gene Expression Profiling; Gene Expression Regulation; Genetic Association Studies; Genetic Diseases, X-Linked; Genetic Therapy; Genetic Variation; Graft Rejection; HeLa Cells; Hematopoietic Stem Cell Transplantation; Histones; Hospitalization; Huntingtin Protein; Huntington Disease; Immunosuppression Therapy; Induced Pluripotent Stem Cells; Inflammation; Inosine; Intermediate Filaments; Intranuclear Inclusion Bodies; Isomerism; Lewy Bodies; Ligases; Liquid Chromatography-Mass Spectrometry; Lysosomes; Medium Spiny Neurons; Methylation; Methyltransferases; Microglia; Microscopy; Microscopy, Electron; Mitochondria; Mitochondrial Proteins; Motor Neurons; Multiomics; Muscle, Skeletal; Mutation; Negotiating; Nervous System Diseases; Neural Stem Cells; Neurites; Neurobiology; Neurodegenerative Diseases; Neurons; Neurons, Efferent; Oligonucleotides, Antisense; Optogenetics; Organelles; Outcome Assessment, Health Care; Parkinson Disease; Peptides; Pharmaceutical Preparations; Phenotype; Pluripotent Stem Cells; Poly Adenosine Diphosphate Ribose; Prevalence; Primates; Prisoners; Promoter Regions, Genetic; Protein Binding; Protein Biosynthesis; Protein Isoforms; Proteins; Proteome; Proteomics; Proteostasis; Quantitative Trait Loci; RNA; RNA Methylation; RNA Splicing; RNA Stability; RNA, Messenger; RNA, Small Interfering; RNA-Binding Proteins; Receptors, Antigen, T-Cell; Receptors, Metabotropic Glutamate; Regenerative Medicine; Registries; Research Report; Retroelements; Robotic Surgical Procedures; SUMO-1 Protein; Salts; Seizures; Seizures, Febrile; Sequence Analysis, RNA; Signal Transduction; Sodium Chloride; Spinocerebellar Ataxias; Stem Cell Transplantation; Stem Cells; Sumoylation; Superoxide Dismutase-1; Synapses; Synapsins; Synaptosomes; Synucleins; Systems Biology; Tandem Mass Spectrometry; Tandem Repeat Sequences; Terminology as Topic; Tissue Distribution; Transcription, Genetic; Transcriptome; Translational Science, Biomedical; Treatment Outcome; Trinucleotide Repeat Expansion; Trinucleotide Repeats; Ubiquitin; Ubiquitin-Protein Ligases; Whole Genome Sequencing; gamma-Aminobutyric Acid</t>
+          <t>6-methyladenine; Academia; Adenosine; Aged; Algorithms; Alternative Splicing; Alzheimer Disease; Amyotrophic Lateral Sclerosis; Animals, Genetically Modified; Artificial Intelligence; Astrocytes; Ataxin-1; Atrophy; Autophagy; Biological Phenomena; Biomarkers; Biomedical Research; Biotin; Brain; Brain-Derived Neurotrophic Factor; C9orf72 Protein; Calcium Signaling; Caregivers; Case-Control Studies; Cell Death; Cell Differentiation; Cell Line; Cell- and Tissue-Based Therapy; Cells, Cultured; Cerebellum; Cerebral Cortex; Child; Child, Preschool; Chorea; Chromatin; Chromatin Immunoprecipitation Sequencing; Chromatography, Liquid; Clinical Trials, Phase I as Topic; Clustered Regularly Interspaced Short Palindromic Repeats; Cognition; Cognitive Dysfunction; Communication; Corpus Striatum; DNA Breaks, Double-Stranded; DNA Damage; DNA Repair; DNA-Binding Proteins; Deep Learning; Delayed Diagnosis; Dementia; Demography; Depression; Dihydroxyphenylalanine; Disease Progression; Dopaminergic Neurons; Drug Development; Dystonia 3, Torsion, X-Linked; Edema; Electrophysiology; Embryonic Stem Cells; Epigenesis, Genetic; Epigenomics; Epilepsies, Partial; Exons; Feasibility Studies; Fibroblasts; Frontotemporal Dementia; Frontotemporal Lobar Degeneration; Gene Editing; Gene Expression Profiling; Gene Expression Regulation; Gene Knockout Techniques; Genetic Association Studies; Genetic Diseases, X-Linked; Genetic Therapy; Genetic Variation; Graft Rejection; HeLa Cells; Hematopoietic Stem Cell Transplantation; Histones; Hospitalization; Huntingtin Protein; Huntington Disease; Immunosuppression Therapy; Induced Pluripotent Stem Cells; Inflammation; Inosine; Intermediate Filaments; Intranuclear Inclusion Bodies; Isomerism; Lewy Bodies; Ligases; Liquid Chromatography-Mass Spectrometry; Lysosomes; Medium Spiny Neurons; Methylation; Methyltransferases; Microglia; Microscopy; Microscopy, Electron; Mitochondria; Mitochondrial Proteins; Motor Neurons; Multiomics; Muscle, Skeletal; Mutation; Negotiating; Nervous System Diseases; Neural Stem Cells; Neurites; Neurobiology; Neurodegenerative Diseases; Neurons; Neurons, Efferent; Oligonucleotides, Antisense; Optogenetics; Organelles; Outcome Assessment, Health Care; Parkinson Disease; Peptides; Pharmaceutical Preparations; Phenotype; Pluripotent Stem Cells; Poly Adenosine Diphosphate Ribose; Prevalence; Primates; Prisoners; Promoter Regions, Genetic; Protein Binding; Protein Biosynthesis; Protein Isoforms; Proteins; Proteome; Proteomics; Proteostasis; Quantitative Trait Loci; RNA; RNA Methylation; RNA Splicing; RNA Stability; RNA, Messenger; RNA, Small Interfering; RNA-Binding Proteins; Receptors, Antigen, T-Cell; Receptors, Metabotropic Glutamate; Regenerative Medicine; Registries; Research Report; Retroelements; Robotic Surgical Procedures; SUMO-1 Protein; Salts; Seizures; Seizures, Febrile; Sequence Analysis, RNA; Signal Transduction; Sodium Chloride; Spinocerebellar Ataxias; Stem Cell Transplantation; Stem Cells; Sumoylation; Superoxide Dismutase-1; Synapses; Synapsins; Synaptosomes; Synucleins; Systems Biology; Tandem Mass Spectrometry; Tandem Repeat Sequences; Terminology as Topic; Tissue Distribution; Transcription, Genetic; Transcriptome; Translational Science, Biomedical; Treatment Outcome; Trinucleotide Repeat Expansion; Trinucleotide Repeats; Ubiquitin; Ubiquitin-Protein Ligases; Whole Genome Sequencing; gamma-Aminobutyric Acid</t>
         </is>
       </c>
     </row>
@@ -1721,7 +1725,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>AMP-Activated Protein Kinases; Acetylation; Adaptor Proteins, Signal Transducing; Adenocarcinoma of Lung; Adolescent; Antineoplastic Agents; Apoptosis; Autophagy; Autophagy-Related Protein 8 Family; B7-H1 Antigen; Blastocyst; Body Patterning; Brain; Breast Neoplasms; Calmodulin-Binding Proteins; Carcinogenesis; Cell Differentiation; Cell Line, Tumor; Cell Proliferation; Cell Survival; Cell Transformation, Neoplastic; Child; Chromatin; Cues; DNA-Binding Proteins; Drosophila Proteins; Drug Resistance, Neoplasm; Dynactin Complex; Dyneins; Embryonic Development; Endoderm; Ependymoma; Fertilization; Florida; Gene Expression Regulation, Developmental; Gene Expression Regulation, Neoplastic; Gene Regulatory Networks; Genes, Neurofibromatosis 2; Genes, Regulator; Genetic Background; Glucose; Glycogen Synthase Kinase 3 beta; Glycosylation; Head and Neck Neoplasms; Hippo Signaling Pathway; Histone Deacetylase 1; Histone Deacetylase 2; Histone Deacetylases; Histones; Homeostasis; Immunity, Innate; Immunotherapy; Inflammation; Intercellular Signaling Peptides and Proteins; Interdisciplinary Research; Intracellular Signaling Peptides and Proteins; Kinesins; Lipids; Loss of Function Mutation; Lung Neoplasms; MAP Kinase Signaling System; Mass Spectrometry; Meningeal Neoplasms; Meningioma; Metabolic Networks and Pathways; Metals, Heavy; Microtubule-Associated Proteins; Microtubules; Morbidity; Mutation; Mutation, Missense; N-Myc Proto-Oncogene Protein; Neoplasms; Neurilemmoma; Neurofibromatosis 2; Neurofibromin 2; Organ Size; Organelles; Phosphoric Monoester Hydrolases; Phosphorylation; Physiological Phenomena; Platinum Compounds; Protein Interaction Mapping; Protein Interaction Maps; Protein Serine-Threonine Kinases; Proteins; Proteomics; Publishing; Pyridines; RNA, Long Noncoding; Receptor, Notch1; Regeneration; Sequence Deletion; Serine; Serine-Threonine Kinase 3; Signal Transduction; Stem Cells; TEA Domain Transcription Factors; Transcription Factor MTF-1; Transcription Factors; Tumor Escape; Tumor Suppressor Proteins; Ubiquitin-Protein Ligases; Ubiquitination; Writing; Xenograft Model Antitumor Assays; nan</t>
+          <t>AMP-Activated Protein Kinases; Acetylation; Adaptor Proteins, Signal Transducing; Adenocarcinoma of Lung; Adolescent; Antineoplastic Agents; Apoptosis; Autophagy; Autophagy-Related Protein 8 Family; B7-H1 Antigen; Biological Phenomena; Blastocyst; Body Patterning; Brain; Breast Neoplasms; Calmodulin-Binding Proteins; Carcinogenesis; Cell Differentiation; Cell Line, Tumor; Cell Proliferation; Cell Survival; Cell Transformation, Neoplastic; Child; Chromatin; Cues; DNA-Binding Proteins; Drosophila Proteins; Drug Resistance, Neoplasm; Dynactin Complex; Dyneins; Embryonic Development; Endoderm; Ependymoma; Fertilization; Florida; Gene Expression; Gene Expression Regulation, Developmental; Gene Expression Regulation, Neoplastic; Gene Regulatory Networks; Genes, Neurofibromatosis 2; Genes, Regulator; Genetic Background; Glucose; Glycogen Synthase Kinase 3 beta; Glycosylation; Head and Neck Neoplasms; Hippo Signaling Pathway; Histone Deacetylase 1; Histone Deacetylase 2; Histone Deacetylases; Histones; Homeostasis; Immunity, Innate; Immunotherapy; Inflammation; Intercellular Signaling Peptides and Proteins; Interdisciplinary Research; Intracellular Signaling Peptides and Proteins; Kinesins; Lipids; Loss of Function Mutation; Lung Neoplasms; MAP Kinase Signaling System; Mass Spectrometry; Meningeal Neoplasms; Meningioma; Metabolic Networks and Pathways; Metals, Heavy; Microtubule-Associated Proteins; Microtubules; Morbidity; Mutation; Mutation, Missense; N-Myc Proto-Oncogene Protein; Neoplasms; Neurilemmoma; Neurofibromatosis 2; Neurofibromin 2; Organ Size; Organelles; Ovarian Neoplasms; Phosphoric Monoester Hydrolases; Phosphorylation; Physiological Phenomena; Platinum; Protein Interaction Mapping; Protein Interaction Maps; Protein Serine-Threonine Kinases; Proteins; Proteomics; Publishing; Pyridines; RNA, Long Noncoding; Receptor, Notch1; Regeneration; Sequence Deletion; Serine; Serine-Threonine Kinase 3; Signal Transduction; Stem Cells; TEA Domain Transcription Factors; Transcription Factors; Tumor Escape; Tumor Suppressor Proteins; Ubiquitin-Protein Ligases; Ubiquitination; Writing; Xenograft Model Antitumor Assays</t>
         </is>
       </c>
     </row>
@@ -1757,7 +1761,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Animals, Genetically Modified; Animals, Wild; Anti-Bacterial Agents; Anti-Inflammatory Agents; Antioxidants; Bacteria; Bacterial Physiological Phenomena; Bacterial Proteins; Bacteriophages; Biological Evolution; Chromosomes; Climate Change; DNA Damage; Diabetes Mellitus; Disease Transmission, Infectious; Drug Resistance, Microbial; Ecology; Ecosystem; Escherichia coli; Evolution, Molecular; Feasibility Studies; Food Supply; Gastrointestinal Microbiome; Gastrointestinal Motility; Gene Flow; Gene Transfer, Horizontal; Genetic Engineering; Genetics; Homeostasis; Host Microbial Interactions; Hyperglycemia; Imaging, Three-Dimensional; Immune System; Inflammation; Intestines; Macrophages; Metronidazole; Microbial Consortia; Microbiology; Microbiota; Motivation; Nitroreductases; Oxidation-Reduction; Peptides; Planets; Predatory Behavior; Public Health; Reactive Oxygen Species; SOS Response, Genetics; Soil; Symbiosis; Synthetic Biology; Systems Biology; Type VI Secretion Systems; Vibrio cholerae; Zebrafish; nan</t>
+          <t>Animals, Genetically Modified; Animals, Wild; Anti-Bacterial Agents; Anti-Inflammatory Agents; Antioxidants; Bacteria; Bacterial Physiological Phenomena; Bacterial Proteins; Bacteriophages; Biological Evolution; Brain; Chromosomes; Climate Change; DNA Damage; Diabetes Mellitus; Disease Transmission, Infectious; Drug Resistance, Microbial; Ecology; Ecosystem; Escherichia coli; Evolution, Molecular; Feasibility Studies; Food Supply; Gastrointestinal Microbiome; Gastrointestinal Motility; Gene Flow; Gene Transfer, Horizontal; Genetic Engineering; Genetics; Homeostasis; Host Microbial Interactions; Hyperglycemia; Imaging, Three-Dimensional; Immune System; Inflammation; Intestines; Macrophages; Metronidazole; Microbial Consortia; Microbiology; Microbiota; Motivation; Nitroreductases; Oxidation-Reduction; Peptides; Planets; Predatory Behavior; Public Health; Reactive Oxygen Species; SOS Response, Genetics; Soil; Symbiosis; Synthetic Biology; Systems Biology; Type VI Secretion Systems; Vibrio cholerae; Virion; Zebrafish</t>
         </is>
       </c>
     </row>
@@ -1769,7 +1773,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Acetate-CoA Ligase; Acetyl Coenzyme A; Acetylation; Activin Receptors, Type I; Adverse Childhood Experiences; Aging; Alzheimer Disease; Amyloid beta-Peptides; Antibodies; Anxiety; Autism Spectrum Disorder; Blotting, Western; Brain; Brain Neoplasms; Brain-Derived Neurotrophic Factor; Calcium; Censuses; Child; Chin; Cholinergic Agents; Cholinergic Neurons; Chromatin; Chromatin Immunoprecipitation; Circadian Rhythm; Cocaine; Cognition; Color Vision Defects; Conditioning, Classical; Cues; Cuprizone; DNA; DNA Methylation; DNA-Binding Proteins; Demyelinating Diseases; Dopaminergic Neurons; Drug-Seeking Behavior; Entropy; Epigenesis, Genetic; Epigenetic Memory; Epigenomics; Fear; Gene Expression; Gene Expression Profiling; Gene Expression Regulation; Gene Regulatory Networks; Genes, X-Linked; Genetic Variation; Genetics; Genomics; Habenula; High-Throughput Nucleotide Sequencing; Hippocampus; Histone Code; Histones; Immunohistochemistry; Intellectual Disability; Interneurons; Jumonji Domain-Containing Histone Demethylases; Leucine Zippers; Life Change Events; Long-Term Potentiation; Longevity; Mass Spectrometry; Medium Spiny Neurons; Membrane Glycoproteins; Memory; Memory Consolidation; Memory, Long-Term; Mental Disorders; Mental Health; Microglia; Mutation; N-nitrosoiminodiacetic acid; Neurodegenerative Diseases; Neurogenesis; Neuroglia; Neuroinflammatory Diseases; Neuronal Plasticity; Neurons; Neurosciences; Nicotine; Nucleosomes; Nucleus Accumbens; Occupations; Pharmaceutical Preparations; Physical Conditioning, Animal; Plaque, Amyloid; Polyadenylation; Polymerase Chain Reaction; Promoter Regions, Genetic; Proteomics; RNA Splicing; RNA, Catalytic; RNA, Messenger; RNA-Binding Proteins; Radiation Dose Hypofractionation; Radiation Exposure; Radiotherapy; Radiotherapy Dosage; Receptors, Immunologic; Recurrence; Reproducibility of Results; Resilience, Psychological; Reward; Sequence Analysis, RNA; Sleep; Spatial Memory; Substance-Related Disorders; Synapses; Synaptic Transmission; Trans-Activators; Transcription Factors; Transcriptome; Wood; X Chromosome; histone deacetylase 3; nan</t>
+          <t>Acetate-CoA Ligase; Acetyl Coenzyme A; Acetylation; Activin Receptors, Type I; Adverse Childhood Experiences; Aging; Alzheimer Disease; Amyloid beta-Peptides; Antibodies; Anxiety; Autism Spectrum Disorder; Blotting, Western; Brain; Brain Neoplasms; Brain-Derived Neurotrophic Factor; Calcium; Cannabinoids; Cannabis; Censuses; Child; Chin; Cholinergic Agents; Cholinergic Neurons; Chromatin; Chromatin Immunoprecipitation; Cocaine; Cocaine-Related Disorders; Cognition; Color Vision Defects; Conditioning, Classical; Conditioning, Operant; Cues; Cuprizone; DNA; DNA Methylation; DNA-Binding Proteins; Delivery of Health Care; Demyelinating Diseases; Dopamine Uptake Inhibitors; Dopaminergic Neurons; Drug-Seeking Behavior; Epigenesis, Genetic; Epigenetic Memory; Epigenomics; Fear; Gastrin-Secreting Cells; Gene Expression; Gene Expression Profiling; Gene Expression Regulation; Gene Regulatory Networks; Genes, X-Linked; Genetic Variation; Genetics; Genomics; Habenula; High-Throughput Nucleotide Sequencing; Hippocampus; Histone Code; Histone Deacetylases; Histones; Immunohistochemistry; Intellectual Disability; Interneurons; Jumonji Domain-Containing Histone Demethylases; Leucine Zippers; Life Change Events; Long-Term Potentiation; Longevity; Mass Spectrometry; Medium Spiny Neurons; Membrane Glycoproteins; Memory; Memory Consolidation; Memory, Long-Term; Microglia; Mutation; N-nitrosoiminodiacetic acid; Neurodegenerative Diseases; Neurogenesis; Neuroglia; Neuroinflammatory Diseases; Neuronal Plasticity; Neurons; Neurosciences; Nicotine; Nucleosomes; Nucleus Accumbens; Occupations; Pharmaceutical Preparations; Physical Conditioning, Animal; Plaque, Amyloid; Point Mutation; Polyadenylation; Polymerase Chain Reaction; Promoter Regions, Genetic; Proteomics; Psychiatry; Public Health; RNA Splicing; RNA, Catalytic; RNA, Messenger; RNA-Binding Proteins; Radiation Dose Hypofractionation; Radiation Exposure; Radiotherapy; Radiotherapy Dosage; Receptors, Immunologic; Recurrence; Reproducibility of Results; Resilience, Psychological; Reward; Schools; Self Administration; Sequence Analysis, RNA; Spatial Memory; Speech; Substance-Related Disorders; Synapses; Synaptic Transmission; Trans-Activators; Transcription Factors; Transcriptome; Wood; X Chromosome; histone deacetylase 3; hydrogen sulfite</t>
         </is>
       </c>
     </row>
@@ -1781,7 +1785,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Bacteria; Coculture Techniques; Gastrointestinal Microbiome; Microbiota; Phylogeny</t>
+          <t>Bacteria; Coculture Techniques; Ecosystem; Gastrointestinal Microbiome; Microbiota; Phylogeny; Population Density; Ruminants</t>
         </is>
       </c>
     </row>
@@ -1793,319 +1797,11 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Adolescent; Adverse Childhood Experiences; Age Factors; Aged; Aged, 80 and over; Aging; Alzheimer Disease; Amygdala; Amyloid; Amyloid beta-Peptides; Anhedonia; Aniline Compounds; Anniversaries and Special Events; Anxiety; Artificial Intelligence; Biological Specimen Banks; Biomarkers; Brain; Cerebrovascular Disorders; Child; Clinical Trials as Topic; Cognition; Cognitive Dysfunction; Cohort Studies; Community-Institutional Relations; Compulsive Behavior; Computational Biology; Computer Simulation; Consensus; Data Aggregation; Data Collection; Data Management; Data Science; Dementia; Depression; Discrimination, Psychological; Documentation; Down Syndrome; Drug Discovery; Ecosystem; Electrophysiological Phenomena; Emotions; Entorhinal Cortex; Exercise; Financial Management; Frontal Lobe; Gamma Rhythm; Head; Hippocampus; Infant, Newborn; Interdisciplinary Research; Interneurons; Learning; Longitudinal Studies; Machine Learning; Magnetic Resonance Imaging; Memory; Memory Consolidation; Memory Disorders; Memory, Episodic; Mental Disorders; Mental Recall; Metadata; Midline Thalamic Nuclei; Motivation; Neocortex; Nervous System Diseases; Neural Pathways; Neuroimaging; Neurophysiology; Neuropsychological Tests; Neuropsychology; Nucleus Accumbens; Oceans and Seas; Pattern Recognition, Physiological; Peptide Fragments; Phenotype; Physicians; Policy; Polyethylene Terephthalates; Polysomnography; Positron-Emission Tomography; Prefrontal Cortex; Premature Birth; Primates; Prospective Studies; Proteostasis Deficiencies; Psychiatry; Publishing; Quality of Life; Reward; Risk Factors; Saliva; Sleep; Software; Spectrum Analysis; Stress Disorders, Post-Traumatic; Surveys and Questionnaires; Temporal Lobe; Theta Rhythm; UK Biobank; Wakefulness; White Matter; Writing; Young Adult; tau Proteins</t>
+          <t>Adolescent; Adverse Childhood Experiences; Age Factors; Aged; Aged, 80 and over; Aging; Alzheimer Disease; Amygdala; Amyloid; Amyloid beta-Peptides; Anhedonia; Aniline Compounds; Anniversaries and Special Events; Anxiety; Artificial Intelligence; Biological Specimen Banks; Biomarkers; Brain; Cerebral Small Vessel Diseases; Cerebrovascular Disorders; Child; Clinical Trials as Topic; Cognition; Cognitive Dysfunction; Cohort Studies; Community-Institutional Relations; Compulsive Behavior; Computational Biology; Computer Simulation; Consensus; Data Aggregation; Data Collection; Data Management; Data Science; Dementia; Depression; Discrimination, Psychological; Documentation; Down Syndrome; Drug Discovery; Ecosystem; Electrophysiological Phenomena; Emotions; Entorhinal Cortex; Exercise; Financial Management; Frontal Lobe; Gamma Rhythm; Head; Hippocampus; Hypoxia; Infant, Newborn; Interdisciplinary Research; Interneurons; Learning; Longitudinal Studies; Machine Learning; Magnetic Resonance Imaging; Memory; Memory Consolidation; Memory Disorders; Memory, Episodic; Mental Disorders; Mental Recall; Metadata; Midline Thalamic Nuclei; Motivation; Neocortex; Nervous System Diseases; Neural Pathways; Neuroimaging; Neurophysiology; Neuropsychological Tests; Neuropsychology; Nucleus Accumbens; Oceans and Seas; Pattern Recognition, Physiological; Peptide Fragments; Phenotype; Physicians; Policy; Polyethylene Terephthalates; Polysomnography; Positron-Emission Tomography; Prefrontal Cortex; Premature Birth; Primates; Prospective Studies; Proteostasis Deficiencies; Psychiatry; Publishing; Quality of Life; Reward; Risk Factors; Saliva; Sleep; Sleep Apnea, Obstructive; Software; Spectrum Analysis; Stress Disorders, Post-Traumatic; Surveys and Questionnaires; Temporal Lobe; Theta Rhythm; UK Biobank; Wakefulness; White Matter; Writing; Young Adult; tau Proteins</t>
         </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002B87155CDAEBE54E8A991CDFF09FE870" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="07d22f826efb92a1b7f7a52cdc9ab0c0">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ccd2e96c-ba06-41a4-9d14-ee5d4767a409" xmlns:ns3="b238fc39-fcbb-4f8c-bfd3-e3a789f7784e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8f50f4dd1661db9c8120150ec829b0b2" ns2:_="" ns3:_="">
-    <xsd:import namespace="ccd2e96c-ba06-41a4-9d14-ee5d4767a409"/>
-    <xsd:import namespace="b238fc39-fcbb-4f8c-bfd3-e3a789f7784e"/>
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all>
-                <xsd:element ref="ns2:SharedWithUsers" minOccurs="0"/>
-                <xsd:element ref="ns2:SharedWithDetails" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceAutoKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceAutoTags" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaLengthInSeconds" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceLocation" minOccurs="0"/>
-                <xsd:element ref="ns3:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
-                <xsd:element ref="ns2:TaxCatchAll" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceObjectDetectorVersions" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceSearchProperties" minOccurs="0"/>
-                <xsd:element ref="ns3:ProjectRole" minOccurs="0"/>
-                <xsd:element ref="ns3:Notes" minOccurs="0"/>
-              </xsd:all>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="ccd2e96c-ba06-41a4-9d14-ee5d4767a409" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="8" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:UserMulti">
-            <xsd:sequence>
-              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
-                <xsd:complexType>
-                  <xsd:sequence>
-                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
-                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
-                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
-                  </xsd:sequence>
-                </xsd:complexType>
-              </xsd:element>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="9" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TaxCatchAll" ma:index="23" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{5edd41bb-06d5-49d8-8697-11a388b6c936}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="ccd2e96c-ba06-41a4-9d14-ee5d4767a409">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="b238fc39-fcbb-4f8c-bfd3-e3a789f7784e" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="10" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="11" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="12" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceKeyPoints" ma:index="13" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceAutoTags" ma:index="14" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="15" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="16" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="17" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="18" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaLengthInSeconds" ma:index="19" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceLocation" ma:index="20" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="22" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="733ad1a4-bcb6-4664-8873-2816a39d1396" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="24" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:description="" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceSearchProperties" ma:index="25" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="ProjectRole" ma:index="26" nillable="true" ma:displayName="Project Role" ma:format="Dropdown" ma:internalName="ProjectRole">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Choice">
-          <xsd:enumeration value="Senior/Key Person"/>
-          <xsd:enumeration value="Other Personnel"/>
-          <xsd:enumeration value="Advisory Board"/>
-          <xsd:enumeration value="Evaluator"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="Notes" ma:index="27" nillable="true" ma:displayName="Notes" ma:format="Dropdown" ma:internalName="Notes">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <ProjectRole xmlns="b238fc39-fcbb-4f8c-bfd3-e3a789f7784e" xsi:nil="true"/>
-    <Notes xmlns="b238fc39-fcbb-4f8c-bfd3-e3a789f7784e" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b238fc39-fcbb-4f8c-bfd3-e3a789f7784e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="ccd2e96c-ba06-41a4-9d14-ee5d4767a409" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34E84BF1-5F9B-4096-B936-0D48D7C5F545}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17A7E850-9D4D-44B4-8B9C-953269D84094}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1332A14B-ECB0-424C-8FEF-A4568240472F}"/>
 </file>
</xml_diff>